<commit_message>
doc:: add report template to the robot
</commit_message>
<xml_diff>
--- a/PriceComparisonRobot2/PriceComarisonRobot2/searcresults.xlsx
+++ b/PriceComparisonRobot2/PriceComarisonRobot2/searcresults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="233">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <x:si>
     <x:t>CategoryId</x:t>
   </x:si>
@@ -37,28 +37,40 @@
     <x:t>GeForce RTX 4060</x:t>
   </x:si>
   <x:si>
+    <x:t>INNO3D GeForce RTX 4060 Videókártya, Twin X2, 8 GB GDDR6, 128 bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ft</x:t>
+  </x:si>
+  <x:si>
     <x:t>Gigabyte GeForce RTX 4060 Videókártya, WINDFORCE OC, 8GB GDDR6, 128 bit</x:t>
   </x:si>
   <x:si>
-    <x:t>Ft</x:t>
+    <x:t>Inno3D GeForce RTX4060 8GB DDR6 Compact, Videókártya</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gigabyte GeForce RTX 4060 EAGLE OC Videokártya, 8GB GDDR6, 128bit</x:t>
   </x:si>
   <x:si>
     <x:t>ASUS Dual GeForce RTX 4060 OC videokártya, 8 GB GDDR6, 128-bit</x:t>
   </x:si>
   <x:si>
-    <x:t>Inno3D GeForce RTX4060 8GB DDR6 Compact, Videókártya</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gigabyte GeForce RTX 4060 EAGLE OC Videokártya, 8GB GDDR6, 128bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INNO3D GeForce RTX 4060 Videókártya, Twin X2, 8 GB GDDR6, 128 bit</x:t>
+    <x:t>Videokártya GainWard GeForce RTX 4060 Ghost 8GB GDDR6 128bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSI GeForce RTX® 4060 VENTUS 2X BLACK videokártya, 8GB GDDR6, 128-bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zotac GeForce RTX 4060 8GB DDR6 Twin Edge, Videókártya</x:t>
   </x:si>
   <x:si>
     <x:t>Gainward GeForce RTX 4060 8GB DDR6 Pegasus, NE64060019P1-1070E, Videókártya</x:t>
   </x:si>
   <x:si>
-    <x:t>MSI GeForce RTX® 4060 VENTUS 2X BLACK videokártya, 8GB GDDR6, 128-bit</x:t>
+    <x:t>Videokártya MSI GeForce RTX 4060 AERO ITX OC 8GB GDDR6 128bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PNY Geforce RTX 4060 8GB DDR6 Verto Dual Ventilátor, Videókártya</x:t>
   </x:si>
   <x:si>
     <x:t>GIGABYTE GeForce RTX 4060 OC Low Profile 8GB GDDR6 videokártya</x:t>
@@ -67,124 +79,103 @@
     <x:t>MSI GeForce RTX 4060 VENTUS 2X WHITE 8G OC NVIDIA 8 GB GDDR6 (V516-030R)</x:t>
   </x:si>
   <x:si>
-    <x:t>Videokártya GainWard GeForce RTX 4060 Ghost 8GB GDDR6 128bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PNY Geforce RTX 4060 8GB DDR6 Verto Dual Ventilátor, Videókártya</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zotac GeForce RTX 4060 8GB DDR6 Twin Edge, Videókártya</x:t>
+    <x:t>Palit GeForce RTX 4060 8GB DDR6 Dual, Videókártya</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Videokártya ASUS GeForce RTX 4060 DUAL EVO OC 8GB GDDR6 128-bit DLSS 3.0</x:t>
   </x:si>
   <x:si>
     <x:t>Palit GeForce RTX 4060 8GB StormX videokártya (NE64060019P1-1070F) (NE64060019P1-1070F)</x:t>
   </x:si>
   <x:si>
-    <x:t>Palit GeForce RTX 4060 8GB DDR6 Dual, Videókártya</x:t>
+    <x:t>ASUS Dual GeForce RTX 4060 Videokártya, 8 GB GDDR6, 128 bites</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PNY GeForce RTX 4060 Ti 8GB XLR8 Gaming Verto EPIC-X RGB Triple Fan DLSS 3 videokártya (VCG40608TFXXPB1) (VCG40608TFXXPB1)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Inno3D GeForce RTX4060 8GB DDR6 Twin X2 OC, Videókártya</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Videókártya PNY Technologies GeForce RTX 4060 8GB XLR8 Gaming VERTO EPIC X RGB</x:t>
   </x:si>
   <x:si>
     <x:t>GIGABYTE GeForce RTX 4060 EAGLE OC ICE 8GB GDDR6 128 bites videokártya</x:t>
   </x:si>
   <x:si>
-    <x:t>Videokártya ASUS GeForce RTX 4060 DUAL EVO OC 8GB GDDR6 128-bit DLSS 3.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS Dual GeForce RTX 4060 Videokártya, 8 GB GDDR6, 128 bites</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inno3D GeForce RTX4060 8GB DDR6 Twin X2 OC, Videókártya</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Videokártya Manli GeForce® RTX 4060 8GB GDDR6 128 bites DLSS 3.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PNY GeForce RTX 4060 Ti 8GB XLR8 Gaming Verto EPIC-X RGB Triple Fan DLSS 3 videokártya (VCG40608TFXXPB1) (VCG40608TFXXPB1)</x:t>
+    <x:t>Zotac ZT-D40600H-10M NVIDIA GeForce RTX 4060 8 GB GDDR6</x:t>
   </x:si>
   <x:si>
     <x:t>Dupla MSI GeForce RTX 4060 GAMING X 8GB GDDR6 128 bites videokártya</x:t>
   </x:si>
   <x:si>
-    <x:t>Videokártya MSI GeForce RTX 4060 AERO ITX OC 8GB GDDR6 128bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zotac GeForce RTX 4060 8GB DDR6 Twin Edge OC, Videókártya</x:t>
+    <x:t>MSI GeForce RTX 4060 Ti VENTUS 2X BLACK 8G OC videokártya, 8GB GDDR6, 128 bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Videokártya ASUS GeForce RTX™ 4060 DUAL OC, 8 GB GDDR6, 128 bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Videokártya Gigabyte GeForce RTX 4060 AERO OC, 8GB GDDR6, 128 bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gigabyte GeForce RTX 4060 GAMING OC videokártya, 8GB GDDR6, 128 bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GEFORCE RTX 4060 TI Windforce OC Videokártya, 8 GB GDDR6, 128 bites</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KFA2 GeForce RTX 4060 EX Videokártya, 1-Click OC 8GB GDDR6 128bit, fehér</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PNY GeForce RTX 4060 8GB XLR8 Gaming Verto EPIC-X RGB Overclocked Triple Ventilátor DLSS 3, Videókártya</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE AORUS GeForce RTX 4060 ELITE videokártya, PCI-Ex16x, 8GB GDDR6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KFA2 NVIDIA GeForce RTX4060 Videokártya, 8GB, GDDR6, HDMI, 3xDP, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PALIT GeForce RTX™ 4060Ti StormX videokártya, 8GB, GDDR6, 128-bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 WINDFORCE 8GB GDDR6 128 bites videokártya</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Videókártya INNO3D GeForce RTX 4060 Ti Twin X2 OC, 8GB GDDR6, 128 bit</x:t>
   </x:si>
   <x:si>
     <x:t>INNO3D GeForce RTX 4060 Ti Twin X2 Videókártya, 8 GB GDDR6, 128 bit</x:t>
   </x:si>
   <x:si>
-    <x:t>KFA2 NVIDIA GeForce RTX4060 Videokártya, 8GB, GDDR6, HDMI, 3xDP, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KFA2 GeForce RTX 4060 8GB ( 1-Click OC 2X), Videókártya</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Videokártya Gigabyte GeForce RTX 4060 AERO OC, 8GB GDDR6, 128 bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gigabyte GeForce RTX 4060 GAMING OC videokártya, 8GB GDDR6, 128 bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MSI GeForce RTX 4060 Ti VENTUS 2X BLACK 8G OC videokártya, 8GB GDDR6, 128 bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PNY GeForce RTX 4060 8GB XLR8 Gaming Verto EPIC-X RGB Overclocked Triple Ventilátor DLSS 3, Videókártya</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GEFORCE RTX 4060 TI Windforce OC Videokártya, 8 GB GDDR6, 128 bites</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KFA2 GeForce RTX 4060 EX Videokártya, 1-Click OC 8GB GDDR6 128bit, fehér</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gainward GeForce RTX 4060 Ti Pegasus 8GB GDDR6 videokártya, GDDR6, 128 bit</x:t>
+    <x:t>Gigabyte AORUS AORUS GeForce® RTX™ 4060 ELITE OC videokártya, 8GB GDDR6, 128-bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gigabyte GeForce RTX 4060 Ti GAMING OC videokártya, 8GB GDDR6, 128-bit</x:t>
   </x:si>
   <x:si>
     <x:t>MSI GEFORCE RTX 4060 TI Videókártya, VENTUS 3X 8G OC, 8GB GDDR6X, 128 bit</x:t>
   </x:si>
   <x:si>
-    <x:t>Videókártya INNO3D GeForce RTX 4060 Ti Twin X2 OC, 8GB GDDR6, 128 bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gigabyte GeForce RTX 4060 Ti AERO OC videokártya, 8 GB GDDR6, 128-bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PALIT GeForce RTX™ 4060Ti StormX videokártya, 8GB, GDDR6, 128-bit</x:t>
+    <x:t>ZOTAC GAMING GeForce RTX 4060Ti Twin Edge - graphics card - GeForce RTX 4060 Ti - 8 GB (ZT-D40610E-10M)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Videokártya GIGABYTE GeForce RTX 4060 Ti WINDFORCE OC 8GB GDDR6 128-bit DLSS 3.0</x:t>
   </x:si>
   <x:si>
     <x:t>Videokártya Twin, Inno3D, NVIDIA GeForce RTX4060, 8G, fehér</x:t>
   </x:si>
   <x:si>
-    <x:t>GIGABYTE AORUS GeForce RTX 4060 ELITE videokártya, PCI-Ex16x, 8GB GDDR6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gigabyte GeForce RTX 4060 Ti GAMING OC videokártya, 8GB GDDR6, 128-bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gigabyte GeForce RTX 4060 Ti AORUS ELITE videokártya, 8GB GDDR6, 128-bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Palit GeForce RTX® 4060 Ti DUAL, 8 GB GDDR6 videokártya, 128-bit</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Videokártya GIGABYTE GeForce RTX 4060 Ti WINDFORCE OC 8GB GDDR6 128-bit DLSS 3.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ZOTAC GAMING GeForce RTX 4060Ti Twin Edge - graphics card - GeForce RTX 4060 Ti - 8 GB (ZT-D40610E-10M)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS GeForce RTX® 4060 Ti DUAL Videokártya, 8 GB GDDR6, 128 bites DLSS 3.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PNY GeForce RTX4060 Ti 8GB XLR8 Gaming Verto EPIC-X RGB Triple Ventilátor DLSS 3, Videókártya</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zotac GAMING GeForce RTX 4060 Ti Twin Edge OC NVIDIA 8 GB GDDR6</x:t>
+    <x:t>Videokártya MSI GeForce RTX 4060 GAMING 8GB GDDR6 128bit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Videokártya MSI GeForce RTX 4060 Ti GAMING X SLIM 8GB GDDR6 128bit</x:t>
   </x:si>
   <x:si>
     <x:t>Gigabyte GeForce RTX 4060 Ti Eagle videokártya, 8 GB GDDR6, 128-bit</x:t>
   </x:si>
   <x:si>
-    <x:t>MSI GEFORCE RTX 4060 TI GAMING X Videókártya, 8 GB GDDR6, 128 bit</x:t>
+    <x:t>Gigabyte Videokártya, GeForce RTX 4060 Ti EAGLE OC, 8GB GDDR6, 128 bites</x:t>
   </x:si>
   <x:si>
     <x:t>Intel Core i5-13400F</x:t>
@@ -214,25 +205,43 @@
     <x:t>X-LSWAB SuperLaser i66 Gaming Headset, Sztereó, Hangerőszabályzó, LED, Beépített mikrofon, Cappuccino</x:t>
   </x:si>
   <x:si>
+    <x:t>X-LSWAB SuperLaser i66 Gaming Headset, Sztereó, Hangerőszabályzó, LED, Beépített mikrofon, Jet Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gaming headset Xtrike ME GH-709, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Baldur gaming headset, Rebeltec, mikrofonnal, fekete/piros</x:t>
+  </x:si>
+  <x:si>
     <x:t>SBOX HS-302 Gaming Headset, fekete/szürke</x:t>
   </x:si>
   <x:si>
-    <x:t>X-LSWAB SuperLaser i66 Gaming Headset, Sztereó, Hangerőszabályzó, LED, Beépített mikrofon, Jet Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset Xtrike ME GH-709, fekete</x:t>
+    <x:t>Gaming headset mikrofonnal Defender WARHEAD G-185, GRA, fekete/piros</x:t>
   </x:si>
   <x:si>
     <x:t>Rampage Snopy SN-4488 BLASTOISE gaming headset fekete-piros (22412) (rampage22412)</x:t>
   </x:si>
   <x:si>
+    <x:t>GENESIS ARGON 110 Sztereó Gaming headset Fekete-piros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Meetion HP010 Gaming Headset, 3D hang, PC / XBOX / PS, Zajszűrő mikrofon, Hangerőszabályzó, Többplatformos, Adapter mellékelve, Fekete/narancs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vezeték nélküli gaming headset, LED kijelző, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gaming headset, Sades, Wings 100 Pro, Töltőtok, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ART HERO Gaming Headset Fekete (330418)</x:t>
+  </x:si>
+  <x:si>
     <x:t>Natec Genesis Argon 500 Gaming Headset Fekete Piros</x:t>
   </x:si>
   <x:si>
-    <x:t>Vezeték nélküli gaming headset, LED kijelző, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GENESIS ARGON 110 Sztereó Gaming headset Fekete-piros</x:t>
+    <x:t>Combatwing gaming headset, M180 Pro, mikrofon, univerzális, LED, fekete</x:t>
   </x:si>
   <x:si>
     <x:t>Rampage Snopy SN-8800 GAMETIME gaming headset fekete (35958) (rampage35958)</x:t>
@@ -241,178 +250,148 @@
     <x:t>Nedis GHST100BK Gaming Headset Fekete-Kék</x:t>
   </x:si>
   <x:si>
+    <x:t>Gaming headset H2038U, Havit, Omnidirectional mikrofon, RGB, fehér/fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dareu EH732 gaming headset, USB, RGB, sárga</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Redragon H220 Themis Gaming Headset, Piros megvilágítás, USB és 3,5 mm Jack, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rampage Snopy SN-GX1 ERGO gaming headset fekete-kék (34974) (rampage34974)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Havit H2042d RGB Vezetékes Gaming Headset</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gaming headset, Onikuma, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Onikuma gaming headset mikrofonnal, játékosoknak, RGB LED, fekete/kék</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Onikuma gaming headset, játékosoknak, mikrofonnal, RGB LED, fekete/piros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vezeték nélküli gaming headset K55, Fülbe helyezhető, Bluetooth 5.0, Beépített mikrofon, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Speedlink SL-860000-BK LEGATOS Stereo Gaming Headset, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zalman ZM-HPS300 Gaming headset, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gaming headset i-JMB 3481, jéglámpákkal, fekete</x:t>
+  </x:si>
+  <x:si>
     <x:t>MediaRange gaming headset, USB-kábellel, Surround 5.1, fekete/piros</x:t>
   </x:si>
   <x:si>
-    <x:t>Meetion HP010 Gaming Headset, 3D hang, PC / XBOX / PS, Zajszűrő mikrofon, Hangerőszabályzó, Többplatformos, Adapter mellékelve, Fekete/narancs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Havit H2042d RGB Vezetékes Gaming Headset</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Redragon H220 Themis Gaming Headset, Piros megvilágítás, USB és 3,5 mm Jack, Fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rampage Snopy SN-GX1 ERGO gaming headset fekete-kék (34974) (rampage34974)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset H2038U, Havit, Omnidirectional mikrofon, RGB, fehér/fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Onikuma gaming headset, játékosoknak, mikrofonnal, RGB LED, fekete/piros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Onikuma gaming headset mikrofonnal, játékosoknak, RGB LED, fekete/kék</x:t>
+    <x:t>Gaming headset mikrofonnal G2000, Kotion Mindegyik, LED, fekete/narancs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ART FLASH illuminate Gaming Headset Kék (330409)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gaming headset, Sades, Zpower, 1,2 m, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stereo Gaming Headset V1 Fekete - Nintendo Switch (SWITCHHEADSETV1)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Stereo Gaming Headset V1 zöld/rózsaszín (SWITCHHEADSETV1P+G)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ziumier vezetékes gaming headset mikrofonnal, kompatibilis PC-vel, PS4, PS5, Xbox One, Xbox Series X és S, Switch, 3,5 mm, audio jack, piros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trust GXT 411P Radius Gaming Headset rózsaszín (24362) (trust24362)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marvo HG8941 Gaming Headset, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gaming headset, NGS, PC/PS4/XBoxhoz, fekete/piros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The G-Lab KORP COBALT W gaming headset fehér (KORP-COBALT-W)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Runmus X15 Legend professzionális gaming headset, Total RGB világítás, vezetékes, HD 7.1 surround, háttérzajszűrés, többplatformos, 50 mm-es hangszóró, 102 dB, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Runmus K2Pro professzionális gaming headset mikrofonnal, 7.1 surround HD, háttérzajszűrő mikrofon, LED fénnyel, PC-hez, PS4, Xbox, Nitendo, 50 mm-es hangszóró, 116 dB, álcázás</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Meetion HP021 gaming headset fehér-rózsaszín (MT-HP021WP) (MT-HP021WP)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Meetion HP021 gaming headset fekete-narancs (MT-HP021BO) (MT-HP021)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NOXO Pyre Gaming headset</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Subsonic Pink Power gaming headset rózsaszín (SA5587-A) (SA5587-A)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OMEGA VARR Gaming VH-8010 gaming headset fekete (VH-8010)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Genius 31710007400 HS-G560 gaming headset, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Professzionális gaming headset, Zggzerg, Vezetékes, USB, Mikrofonnal, Led fénnyel, Hangszóró 50mm, Háttérzaj kiszűrése, Széles körű kompatibilitás, PC/Notebook/Telefon/Pad/PS4, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NACON Stereo Gaming Headset V3 PlayStation 4-hez, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rampage Snopy SN-8800 GAMETIME RGB gaming headset fekete (35111) (rampage35111)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tracer BATTLE HEROES Gunman Gaming Headset, kék</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Motospeed H60 gaming headset, beépített 7.1 audio csatorna, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Xtrike Me GH-890 RGB Gaming Headset, fekete/piros</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Meetion HP020 Gaming Headset, 3D hang, RGB világítás, PC-hez / XBOX / PS-hez, Zajszűrő mikrofon, Hangerőszabályzó, Többplatformos, Adapterrel, Fekete/narancssárga</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Easy HellCrack Z11 gaming fekete fejhallgató headset</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Easy HellCrack Z11 gaming Narancs Fejhallgató headset</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Easy HellCrack Z11 gaming Piros Fejhallgató headset</x:t>
   </x:si>
   <x:si>
     <x:t>Redragon Ares RGB Gaming Headset, fekete</x:t>
   </x:si>
   <x:si>
-    <x:t>Gaming headset i-JMB 3481, jéglámpákkal, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset mikrofonnal Defender WARHEAD G-185, GRA, fekete/piros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset mikrofonnal G2000, Kotion Mindegyik, LED, fekete/narancs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Speedlink SL-860000-BK LEGATOS Stereo Gaming Headset, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ART HERO Gaming Headset Fekete (330418)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset, Onikuma, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stereo Gaming Headset V1 Fekete - Nintendo Switch (SWITCHHEADSETV1)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ziumier vezetékes gaming headset mikrofonnal, kompatibilis PC-vel, PS4, PS5, Xbox One, Xbox Series X és S, Switch, 3,5 mm, audio jack, piros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset, NGS, PC/PS4/XBoxhoz, fekete/piros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Marvo HG8941 Gaming Headset, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dareu EH732 gaming headset, USB, RGB, sárga</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Runmus X15 Legend professzionális gaming headset, Total RGB világítás, vezetékes, HD 7.1 surround, háttérzajszűrés, többplatformos, 50 mm-es hangszóró, 102 dB, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Runmus K2Pro professzionális gaming headset mikrofonnal, 7.1 surround HD, háttérzajszűrő mikrofon, LED fénnyel, PC-hez, PS4, Xbox, Nitendo, 50 mm-es hangszóró, 116 dB, álcázás</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Meetion HP021 gaming headset fekete-narancs (MT-HP021BO) (MT-HP021)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trust GXT 411P Radius Gaming Headset rózsaszín (24362) (trust24362)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NOXO Pyre Gaming headset</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Subsonic Pink Power gaming headset rózsaszín (SA5587-A) (SA5587-A)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zalman ZM-HPS300 Gaming headset, Fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OMEGA VARR Gaming VH-8010 gaming headset fekete (VH-8010)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Meetion HP021 gaming headset fehér-rózsaszín (MT-HP021WP) (MT-HP021WP)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset PC-hez, RGB lámpák és mikrofon, hangerőszabályzó, Multicolor, 2 db</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tracer BATTLE HEROES Gunman Gaming Headset, kék</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stereo Gaming Headset V1 zöld/rózsaszín (SWITCHHEADSETV1P+G)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Genius 31710007400 HS-G560 gaming headset, Fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Xtrike Me GH-890 RGB Gaming Headset, fekete/piros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Motospeed H60 gaming headset, beépített 7.1 audio csatorna, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nemezis Gaming Headset, Prémium, mikrofon mellékelve, vezetékkel állítható, fekete/piros színű</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rampage Snopy SN-8800 GAMETIME RGB gaming headset fekete (35111) (rampage35111)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Meetion HP020 Gaming Headset, 3D hang, RGB világítás, PC-hez / XBOX / PS-hez, Zajszűrő mikrofon, Hangerőszabályzó, Többplatformos, Adapterrel, Fekete/narancssárga</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Easy HellCrack Z11 gaming fekete fejhallgató headset</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Easy HellCrack Z11 gaming Narancs Fejhallgató headset</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Easy HellCrack Z11 gaming Piros Fejhallgató headset</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset Trust GXT 415 Zirox, mikrofon, fekete</x:t>
+    <x:t>Gaming headset Edifier K815, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Professzionális gaming headset, Zggzerg, Vezetékes, USB, Mikrofonnal, RGB világítás, Virtuális surround HD, hangszigetelés, háttérzaj kiszűrés, 50 mm-es hangszóró, USB és 3,5 mm-es jack csatlakozó, Multiplatform, Fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Onikuma K1B, PC/PS4/XBOX gaming headset, LED-ek, beépített mikrofon, fekete</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wesdar GH30 gaming headset mikrofonnal</x:t>
   </x:si>
   <x:si>
     <x:t>DELTACO GAMING DH210 vezetékes gamer headset, többplatformos PC/Xbox/PlayStation, fekete/narancs</x:t>
   </x:si>
   <x:si>
-    <x:t>Gaming headset Trust GXT 415P Zirox, mikrofon, rózsaszín</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wesdar GH30 gaming headset mikrofonnal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bigben Stereo Gaming Headset V3, PS4, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset mikrofonnal PS4 PS5 Xbox One PC-hez RGB fényzajszűrő mikrofon basszus térhatású hang laptophoz, Mac Nintendo Switch Playstation Xbox Version Tech</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Onikuma gaming headset, X10, mikrofon, LED, RGB, fekete/ezüst</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gaming headset, Sades, Wings 100 Pro, Töltőtok, Fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stereo Gaming Headset V1 Kék (NSW) (SWITCHHEADSETV1R+B)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stereo Gaming Headset V1 Fekete - XBOX Series (XBXHEADSETV1)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vezetékes 5.1 Likesmart High Tech gaming headset, RGB világítás, tiszta hang, állítható mikrofon, bármilyen fejmérethez állítható, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Patriot PV3607UMLK Viper Virtual 7.1 Gaming Headset Fekete-Piros (342856)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Natec NSG-1578 Genesis Radon 300 7.1 Surround Gaming Headset Fekete-piros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Baldur gaming headset, Rebeltec, mikrofonnal, fekete/piros</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gamdias HEBE E1 Gaming headset, Fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RoXPower T-ROX STGH707 PC Gaming Headset mikrofonnal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Runmus X15 PRO professzionális gaming headset, Total RGB világítás, HD 7.1 surround, háttérzajszűrés, többplatformos, 50 mm-es hangszóró, 102 dB, fekete</x:t>
+    <x:t>Gamdias HEBE E3 RGB Gaming headset, 3.5mm, Fekete</x:t>
   </x:si>
   <x:si>
     <x:t>B650 AORUS</x:t>
@@ -427,24 +406,30 @@
     <x:t>Alaplap GIGABYTE B650M AORUS ELITE AX-ICE, AM5 foglalat, Wi-Fi 6E, DDR5 B650M-A-ELIT-AX-ICE</x:t>
   </x:si>
   <x:si>
+    <x:t>Gigabyte B650 AORUS ELITE AX ICE alaplap, AM5 Socket, ATX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE B650E AORUS ELITE AX ICE alaplap, AM5 Socket, ATX</x:t>
+  </x:si>
+  <x:si>
     <x:t>Alaplap GIGABYTE B650 AORUS ELITE AX V2, AM5, AMD B650, ATX</x:t>
   </x:si>
   <x:si>
+    <x:t>Alaplap Gigabyte B650 AORUS ELITE AX V2 Socket AM5</x:t>
+  </x:si>
+  <x:si>
     <x:t>Gigabyte B650 AORUS ELITE AX ICE, Alaplap</x:t>
   </x:si>
   <x:si>
     <x:t>Alaplap GIGABYTE B650E AORUS ELITE AXE ICE AM5, 4x DDR5, 2x HDMI 1x USB TYPE-C, 3x PCIE x16, 3x</x:t>
   </x:si>
   <x:si>
-    <x:t>Alaplap Gigabyte B650 AORUS ELITE AX V2 Socket AM5</x:t>
+    <x:t>Gigabyte B650I AORUS ULTRA, Alaplap</x:t>
   </x:si>
   <x:si>
     <x:t>GIGABYTE B650 AORUS PRO AX alaplap</x:t>
   </x:si>
   <x:si>
-    <x:t>Gigabyte B650I AORUS ULTRA, Alaplap</x:t>
-  </x:si>
-  <x:si>
     <x:t>GIGABYTE B650E Aorus Master Alaplap</x:t>
   </x:si>
   <x:si>
@@ -454,100 +439,94 @@
     <x:t>LG 27GR95QE-B 27" Gaming monitor, OLED, 16:9, 2560x1440, 240Hz, 0.03ms, 200cd, HDMIx2, DP, USB, G-Sync, HDR, Pivot, Fekete</x:t>
   </x:si>
   <x:si>
+    <x:t>ASUS DUAL GeForce RTX 4060 O8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 EAGLE OC 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 WINDFORCE OC 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ASUS PROART GeForce RTX 4060 O8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 GAMING OC 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSI GeForce RTX 4060 Ti VENTUS 2X BLACK 16G OC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 Ti GAMING OC 16G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ASUS DUAL GeForce RTX 4060 Ti O8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSI GeForce RTX 4060 VENTUS 2X BLACK 8G OC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GAINWARD GeForce RTX 4060 Ti Ghost 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 Ti EAGLE 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ASUS DUAL GeForce RTX 4060 Ti O16G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 Ti GAMING OC 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 Ti WINDFORCE OC 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GAINWARD GeForce RTX 4060 Ghost 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Inno3D GeForce RTX 4060 Ti Twin X2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSI GeForce RTX 4060 Ti GAMING X SLIM 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 Ti AERO OC 16G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE AORUS GeForce RTX 4060 ELITE 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE GeForce RTX 4060 AERO OC 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Inno3D GeForce RTX 4060 Ti Twin X2 OC White</x:t>
+  </x:si>
+  <x:si>
     <x:t>Inno3D GeForce RTX 4060 Twin X2 OC</x:t>
   </x:si>
   <x:si>
+    <x:t>MSI GeForce RTX 4060 VENTUS 2X WHITE 8G OC</x:t>
+  </x:si>
+  <x:si>
     <x:t>GIGABYTE GeForce RTX 4060 D6 8G</x:t>
   </x:si>
   <x:si>
-    <x:t>GAINWARD GeForce RTX 4060 Ghost 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS DUAL GeForce RTX 4060 O8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GeForce RTX 4060 EAGLE OC 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MSI GeForce RTX 4060 VENTUS 2X WHITE 8G OC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS PROART GeForce RTX 4060 O8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GeForce RTX 4060 GAMING OC 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS DUAL GeForce RTX 4060 O8G EVO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS DUAL GeForce RTX 4060 O8G WHITE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MSI GeForce RTX 4060 GAMING X 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inno3D GeForce RTX 4060 Ti Twin X2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GAINWARD GeForce RTX 4060 Ti Ghost 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inno3D GeForce RTX 4060 Ti Twin X2 OC White</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS DUAL GeForce RTX 4060 Ti O8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MSI GeForce RTX 4060 Ti VENTUS 2X BLACK 8G OC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GeForce RTX 4060 WINDFORCE OC 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE AORUS GeForce RTX 4060 ELITE 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GeForce RTX 4060 Ti GAMING OC 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GeForce RTX 4060 Ti EAGLE OC 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GeForce RTX 4060 Ti EAGLE 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MSI GeForce RTX 4060 Ti VENTUS 2X BLACK 16G OC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS DUAL GeForce RTX 4060 Ti O16G</x:t>
+    <x:t>GIGABYTE GeForce RTX 4060 Ti AERO OC 8G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MSI GeForce RTX 4060 Ti GAMING X 16G</x:t>
   </x:si>
   <x:si>
     <x:t>Inno3D GeForce RTX 4060 Ti iChill X3 8G</x:t>
   </x:si>
   <x:si>
-    <x:t>Inno3D GeForce RTX 4060 Ti Twin X2 OC 16G</x:t>
-  </x:si>
-  <x:si>
     <x:t>Inno3D GeForce RTX 4060 Ti iChill X3 8G White</x:t>
   </x:si>
   <x:si>
-    <x:t>MSI GeForce RTX 4060 Ti GAMING X SLIM 8G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE GeForce RTX 4060 Ti GAMING OC 16G</x:t>
-  </x:si>
-  <x:si>
     <x:t>GAINWARD GeForce RTX 4060 Ti Panther 16G</x:t>
   </x:si>
   <x:si>
-    <x:t>MSI GeForce RTX 4060 Ti GAMING X 16G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS ProArt GeForce RTX 4060 Ti O16G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ASUS ROG STRIX GeForce RTX 4060 Ti A16G</x:t>
+    <x:t>ASUS PROART GeForce RTX 4060 Ti 16G</x:t>
   </x:si>
   <x:si>
     <x:t>16 GB DDR5</x:t>
@@ -565,58 +544,79 @@
     <x:t>Crucial SO-DIMM 16GB DDR5 5200MHz CL42</x:t>
   </x:si>
   <x:si>
+    <x:t>Crucial SO-DIMM 16GB DDR5 5600MHz CL46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 5200MHz CL36 Beast White EXPO</x:t>
+  </x:si>
+  <x:si>
     <x:t>Kingston FURY SO-DIMM 16GB DDR5 4800MHz CL38 Impact</x:t>
   </x:si>
   <x:si>
-    <x:t>Crucial SO-DIMM 16GB DDR5 5600MHz CL46</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 5200MHz CL36 Beast White EXPO</x:t>
+    <x:t>Kingston FURY 16GB DDR5 4800MHz CL38 Beast Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 5200MHz CL40 Beast Black</x:t>
   </x:si>
   <x:si>
     <x:t>Kingston SO-DIMM 16GB DDR5 4800MT/s CL40</x:t>
   </x:si>
   <x:si>
+    <x:t>Lexar SO-DIMM 16GB DDR5 4800MHz CL40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crucial SO-DIMM 16GB KIT DDR5 5600MHz CL46</x:t>
+  </x:si>
+  <x:si>
     <x:t>Kingston FURY 16GB DDR5 5600MHz CL40 Beast White XMP</x:t>
   </x:si>
   <x:si>
-    <x:t>Crucial SO-DIMM 16GB KIT DDR5 5600MHz CL46</x:t>
+    <x:t>Crucial SO-DIMM 16GB KIT DDR5 5200MHz CL42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston SO-DIMM 16GB DDR5 4800MHz CL40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 5200MHz CL36 Beast Black EXPO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 5600MHz CL36 Beast White EXPO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ADATA Lancer 16GB DDR5 5200MHz CL38 RGB Black</x:t>
   </x:si>
   <x:si>
     <x:t>Kingston FURY 16GB DDR5 5600MHz CL40 Beast Black</x:t>
   </x:si>
   <x:si>
-    <x:t>Kingston FURY 16GB DDR5 5200MHz CL40 Beast Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Crucial SO-DIMM 16GB KIT DDR5 5200MHz CL42</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 5200MHz CL36 Beast Black EXPO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston SO-DIMM 16GB DDR5 4800MHz CL40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 5600MHz CL36 Beast White EXPO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ADATA Lancer 16GB DDR5 5200MHz CL38 RGB Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 4800MHz CL38 Beast Black</x:t>
+    <x:t>Kingston FURY 16GB DDR5 5200MHz CL40 Beast White XMP</x:t>
   </x:si>
   <x:si>
     <x:t>Kingston FURY 16GB DDR5 6000MHz CL40 Beast White XMP</x:t>
   </x:si>
   <x:si>
+    <x:t>Lexar SO-DIMM 16GB DDR5 5600MHz CL46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB KIT DDR5 5200MHz CL40 Beast Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY SO-DIMM 16GB DDR5 5600MHz CL40 Impact</x:t>
+  </x:si>
+  <x:si>
     <x:t>Kingston FURY 16GB DDR5 6000MHz CL36 Beast White EXPO</x:t>
   </x:si>
   <x:si>
+    <x:t>Kingston FURY SO-DIMM 16GB DDR5 6000MHz CL38 Impact XMP</x:t>
+  </x:si>
+  <x:si>
     <x:t>Kingston FURY 16GB DDR5 5600MHz CL36 Beast Black EXPO</x:t>
   </x:si>
   <x:si>
-    <x:t>Kingston FURY SO-DIMM 16GB DDR5 5600MHz CL40 Impact</x:t>
+    <x:t>Kingston FURY 16GB DDR5 6000MHz CL40 Beast Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 6000MHz CL36 Beast Black EXPO</x:t>
   </x:si>
   <x:si>
     <x:t>Kingston FURY 16GB DDR5 5600MHz CL36 Beast White RGB EXPO</x:t>
@@ -625,49 +625,22 @@
     <x:t>Kingston FURY 16GB DDR5 5600MHz CL36 Beast Black RGB EXPO</x:t>
   </x:si>
   <x:si>
-    <x:t>Kingston FURY 16GB DDR5 5200MHz CL40 Beast White XMP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 5200MHz CL40 Beast Black RGB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB KIT DDR5 5200MHz CL40 Beast Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 6000MHz CL36 Beast Black EXPO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB KIT DDR5 4800MHz CL38 Beast Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 6000MHz CL36 Beast Black RGB EXPO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 6000MHz CL40 Beast Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 5600MHz CL40 Beast Black RGB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY SO-DIMM 16GB DDR5 6000MHz CL38 Impact XMP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB DDR5 6000MHz CL40 Beast Black RGB</x:t>
+    <x:t>Kingston FURY 16GB DDR5 6000MT/s CL30 Beast Black EXPO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 6000MT/s CL30 Beast Black XMP</x:t>
   </x:si>
   <x:si>
     <x:t>Kingston FURY 16GB KIT DDR5 5600MHz CL40 Beast Black</x:t>
   </x:si>
   <x:si>
-    <x:t>Kingston FURY 16GB KIT DDR5 5200MHz CL36 Beast EXPO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kingston FURY 16GB KIT DDR5 6000MHz CL40 Beast Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Logitech G PRO X 2 LIGHTSPEED Gaming Headset, fekete</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Logitech G PRO X 2 LIGHTSPEED Gaming Headset, fehér</x:t>
+    <x:t>Crucial Overclocking Pro 16GB DDR5 6000MHz CL36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 6000MHz CL36 Beast White RGB EXPO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kingston FURY 16GB DDR5 6000MHz CL32 Renegade</x:t>
   </x:si>
   <x:si>
     <x:t>CONNECT IT CHP-4510-BL Gaming Headset BIOHAZARD kék</x:t>
@@ -691,19 +664,16 @@
     <x:t>GIGABYTE B650 AORUS ELITE AX V2</x:t>
   </x:si>
   <x:si>
+    <x:t>GIGABYTE B650E AORUS ELITE X AX ICE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE B650 AORUS ELITE AX ICE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GIGABYTE B650I AORUS ULTRA</x:t>
+  </x:si>
+  <x:si>
     <x:t>GIGABYTE B650 AORUS PRO AX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE B650 AORUS ELITE AX ICE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE B650I AORUS ULTRA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE B650E AORUS ELITE X AX ICE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GIGABYTE B650E AORUS MASTER</x:t>
   </x:si>
   <x:si>
     <x:t>27" LG 27GR95QE-B</x:t>
@@ -1100,7 +1070,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
-        <x:v>130690</x:v>
+        <x:v>131190</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
         <x:v>52</x:v>
@@ -1120,7 +1090,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>134790</x:v>
+        <x:v>132090</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
         <x:v>52</x:v>
@@ -1140,7 +1110,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
-        <x:v>135650</x:v>
+        <x:v>133660</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
         <x:v>52</x:v>
@@ -1160,7 +1130,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>135690</x:v>
+        <x:v>133690</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
         <x:v>52</x:v>
@@ -1180,7 +1150,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>136590</x:v>
+        <x:v>134890</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
         <x:v>52</x:v>
@@ -1200,7 +1170,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D7" s="0" t="n">
-        <x:v>140300</x:v>
+        <x:v>138230</x:v>
       </x:c>
       <x:c r="E7" s="0" t="n">
         <x:v>52</x:v>
@@ -1220,7 +1190,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="D8" s="0" t="n">
-        <x:v>141190</x:v>
+        <x:v>138990</x:v>
       </x:c>
       <x:c r="E8" s="0" t="n">
         <x:v>52</x:v>
@@ -1240,7 +1210,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="D9" s="0" t="n">
-        <x:v>141510</x:v>
+        <x:v>142050</x:v>
       </x:c>
       <x:c r="E9" s="0" t="n">
         <x:v>52</x:v>
@@ -1260,7 +1230,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D10" s="0" t="n">
-        <x:v>142343</x:v>
+        <x:v>142157</x:v>
       </x:c>
       <x:c r="E10" s="0" t="n">
         <x:v>52</x:v>
@@ -1280,7 +1250,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="D11" s="0" t="n">
-        <x:v>143360</x:v>
+        <x:v>142650</x:v>
       </x:c>
       <x:c r="E11" s="0" t="n">
         <x:v>52</x:v>
@@ -1300,7 +1270,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D12" s="0" t="n">
-        <x:v>145330</x:v>
+        <x:v>143780</x:v>
       </x:c>
       <x:c r="E12" s="0" t="n">
         <x:v>52</x:v>
@@ -1320,7 +1290,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="D13" s="0" t="n">
-        <x:v>147650</x:v>
+        <x:v>144250</x:v>
       </x:c>
       <x:c r="E13" s="0" t="n">
         <x:v>52</x:v>
@@ -1340,7 +1310,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="D14" s="0" t="n">
-        <x:v>150136</x:v>
+        <x:v>144880</x:v>
       </x:c>
       <x:c r="E14" s="0" t="n">
         <x:v>52</x:v>
@@ -1360,7 +1330,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="D15" s="0" t="n">
-        <x:v>150258</x:v>
+        <x:v>147160</x:v>
       </x:c>
       <x:c r="E15" s="0" t="n">
         <x:v>52</x:v>
@@ -1380,7 +1350,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="D16" s="0" t="n">
-        <x:v>150890</x:v>
+        <x:v>148661</x:v>
       </x:c>
       <x:c r="E16" s="0" t="n">
         <x:v>52</x:v>
@@ -1400,7 +1370,7 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="D17" s="0" t="n">
-        <x:v>151020</x:v>
+        <x:v>149602</x:v>
       </x:c>
       <x:c r="E17" s="0" t="n">
         <x:v>52</x:v>
@@ -1420,7 +1390,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="D18" s="0" t="n">
-        <x:v>151240</x:v>
+        <x:v>150780</x:v>
       </x:c>
       <x:c r="E18" s="0" t="n">
         <x:v>52</x:v>
@@ -1440,7 +1410,7 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="D19" s="0" t="n">
-        <x:v>154510</x:v>
+        <x:v>152640</x:v>
       </x:c>
       <x:c r="E19" s="0" t="n">
         <x:v>52</x:v>
@@ -1460,7 +1430,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="D20" s="0" t="n">
-        <x:v>154626</x:v>
+        <x:v>153747</x:v>
       </x:c>
       <x:c r="E20" s="0" t="n">
         <x:v>52</x:v>
@@ -1480,7 +1450,7 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="D21" s="0" t="n">
-        <x:v>155860</x:v>
+        <x:v>156568</x:v>
       </x:c>
       <x:c r="E21" s="0" t="n">
         <x:v>52</x:v>
@@ -1500,7 +1470,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="D22" s="0" t="n">
-        <x:v>155920</x:v>
+        <x:v>156910</x:v>
       </x:c>
       <x:c r="E22" s="0" t="n">
         <x:v>52</x:v>
@@ -1520,7 +1490,7 @@
         <x:v>29</x:v>
       </x:c>
       <x:c r="D23" s="0" t="n">
-        <x:v>156207</x:v>
+        <x:v>156961</x:v>
       </x:c>
       <x:c r="E23" s="0" t="n">
         <x:v>52</x:v>
@@ -1540,7 +1510,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="D24" s="0" t="n">
-        <x:v>157055</x:v>
+        <x:v>157165</x:v>
       </x:c>
       <x:c r="E24" s="0" t="n">
         <x:v>52</x:v>
@@ -1560,7 +1530,7 @@
         <x:v>31</x:v>
       </x:c>
       <x:c r="D25" s="0" t="n">
-        <x:v>160190</x:v>
+        <x:v>158890</x:v>
       </x:c>
       <x:c r="E25" s="0" t="n">
         <x:v>52</x:v>
@@ -1580,7 +1550,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="D26" s="0" t="n">
-        <x:v>162147</x:v>
+        <x:v>161296</x:v>
       </x:c>
       <x:c r="E26" s="0" t="n">
         <x:v>52</x:v>
@@ -1600,7 +1570,7 @@
         <x:v>33</x:v>
       </x:c>
       <x:c r="D27" s="0" t="n">
-        <x:v>163371</x:v>
+        <x:v>162970</x:v>
       </x:c>
       <x:c r="E27" s="0" t="n">
         <x:v>52</x:v>
@@ -1620,7 +1590,7 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="D28" s="0" t="n">
-        <x:v>164370</x:v>
+        <x:v>164604</x:v>
       </x:c>
       <x:c r="E28" s="0" t="n">
         <x:v>52</x:v>
@@ -1640,7 +1610,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="D29" s="0" t="n">
-        <x:v>164604</x:v>
+        <x:v>165190</x:v>
       </x:c>
       <x:c r="E29" s="0" t="n">
         <x:v>52</x:v>
@@ -1660,7 +1630,7 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="D30" s="0" t="n">
-        <x:v>168390</x:v>
+        <x:v>168274</x:v>
       </x:c>
       <x:c r="E30" s="0" t="n">
         <x:v>52</x:v>
@@ -1680,7 +1650,7 @@
         <x:v>37</x:v>
       </x:c>
       <x:c r="D31" s="0" t="n">
-        <x:v>169725</x:v>
+        <x:v>168655</x:v>
       </x:c>
       <x:c r="E31" s="0" t="n">
         <x:v>52</x:v>
@@ -1700,7 +1670,7 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="D32" s="0" t="n">
-        <x:v>170790</x:v>
+        <x:v>171490</x:v>
       </x:c>
       <x:c r="E32" s="0" t="n">
         <x:v>52</x:v>
@@ -1720,7 +1690,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="D33" s="0" t="n">
-        <x:v>173176</x:v>
+        <x:v>171950</x:v>
       </x:c>
       <x:c r="E33" s="0" t="n">
         <x:v>52</x:v>
@@ -1740,7 +1710,7 @@
         <x:v>40</x:v>
       </x:c>
       <x:c r="D34" s="0" t="n">
-        <x:v>173410</x:v>
+        <x:v>172470</x:v>
       </x:c>
       <x:c r="E34" s="0" t="n">
         <x:v>52</x:v>
@@ -1760,7 +1730,7 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="D35" s="0" t="n">
-        <x:v>176390</x:v>
+        <x:v>174341</x:v>
       </x:c>
       <x:c r="E35" s="0" t="n">
         <x:v>52</x:v>
@@ -1780,7 +1750,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="D36" s="0" t="n">
-        <x:v>177080</x:v>
+        <x:v>174970</x:v>
       </x:c>
       <x:c r="E36" s="0" t="n">
         <x:v>52</x:v>
@@ -1800,7 +1770,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="D37" s="0" t="n">
-        <x:v>180390</x:v>
+        <x:v>174970</x:v>
       </x:c>
       <x:c r="E37" s="0" t="n">
         <x:v>52</x:v>
@@ -1820,7 +1790,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="D38" s="0" t="n">
-        <x:v>180610</x:v>
+        <x:v>175690</x:v>
       </x:c>
       <x:c r="E38" s="0" t="n">
         <x:v>52</x:v>
@@ -1840,7 +1810,7 @@
         <x:v>45</x:v>
       </x:c>
       <x:c r="D39" s="0" t="n">
-        <x:v>181265</x:v>
+        <x:v>176390</x:v>
       </x:c>
       <x:c r="E39" s="0" t="n">
         <x:v>52</x:v>
@@ -1860,7 +1830,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="D40" s="0" t="n">
-        <x:v>182390</x:v>
+        <x:v>176490</x:v>
       </x:c>
       <x:c r="E40" s="0" t="n">
         <x:v>52</x:v>
@@ -1880,7 +1850,7 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="D41" s="0" t="n">
-        <x:v>182990</x:v>
+        <x:v>178140</x:v>
       </x:c>
       <x:c r="E41" s="0" t="n">
         <x:v>52</x:v>
@@ -1900,7 +1870,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="D42" s="0" t="n">
-        <x:v>184390</x:v>
+        <x:v>178990</x:v>
       </x:c>
       <x:c r="E42" s="0" t="n">
         <x:v>52</x:v>
@@ -1920,7 +1890,7 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="D43" s="0" t="n">
-        <x:v>185970</x:v>
+        <x:v>181265</x:v>
       </x:c>
       <x:c r="E43" s="0" t="n">
         <x:v>52</x:v>
@@ -1940,7 +1910,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="D44" s="0" t="n">
-        <x:v>188320</x:v>
+        <x:v>182834</x:v>
       </x:c>
       <x:c r="E44" s="0" t="n">
         <x:v>52</x:v>
@@ -1960,7 +1930,7 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="D45" s="0" t="n">
-        <x:v>188860</x:v>
+        <x:v>183290</x:v>
       </x:c>
       <x:c r="E45" s="0" t="n">
         <x:v>52</x:v>
@@ -1980,7 +1950,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="D46" s="0" t="n">
-        <x:v>189360</x:v>
+        <x:v>183920</x:v>
       </x:c>
       <x:c r="E46" s="0" t="n">
         <x:v>52</x:v>
@@ -2000,7 +1970,7 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="D47" s="0" t="n">
-        <x:v>189780</x:v>
+        <x:v>187020</x:v>
       </x:c>
       <x:c r="E47" s="0" t="n">
         <x:v>52</x:v>
@@ -2011,16 +1981,16 @@
     </x:row>
     <x:row r="48" spans="1:6">
       <x:c r="A48" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D48" s="0" t="n">
-        <x:v>191940</x:v>
+        <x:v>77990</x:v>
       </x:c>
       <x:c r="E48" s="0" t="n">
         <x:v>52</x:v>
@@ -2031,16 +2001,16 @@
     </x:row>
     <x:row r="49" spans="1:6">
       <x:c r="A49" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D49" s="0" t="n">
-        <x:v>192970</x:v>
+        <x:v>85294</x:v>
       </x:c>
       <x:c r="E49" s="0" t="n">
         <x:v>52</x:v>
@@ -2051,16 +2021,16 @@
     </x:row>
     <x:row r="50" spans="1:6">
       <x:c r="A50" s="0" t="n">
-        <x:v>192</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D50" s="0" t="n">
-        <x:v>193690</x:v>
+        <x:v>3088</x:v>
       </x:c>
       <x:c r="E50" s="0" t="n">
         <x:v>52</x:v>
@@ -2071,16 +2041,16 @@
     </x:row>
     <x:row r="51" spans="1:6">
       <x:c r="A51" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D51" s="0" t="n">
-        <x:v>78390</x:v>
+        <x:v>3309</x:v>
       </x:c>
       <x:c r="E51" s="0" t="n">
         <x:v>52</x:v>
@@ -2091,16 +2061,16 @@
     </x:row>
     <x:row r="52" spans="1:6">
       <x:c r="A52" s="0" t="n">
-        <x:v>187</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
         <x:v>57</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D52" s="0" t="n">
-        <x:v>90459</x:v>
+        <x:v>3390</x:v>
       </x:c>
       <x:c r="E52" s="0" t="n">
         <x:v>52</x:v>
@@ -2114,13 +2084,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
         <x:v>61</x:v>
       </x:c>
       <x:c r="D53" s="0" t="n">
-        <x:v>3122</x:v>
+        <x:v>3685</x:v>
       </x:c>
       <x:c r="E53" s="0" t="n">
         <x:v>52</x:v>
@@ -2134,13 +2104,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
       <x:c r="D54" s="0" t="n">
-        <x:v>3309</x:v>
+        <x:v>3685</x:v>
       </x:c>
       <x:c r="E54" s="0" t="n">
         <x:v>52</x:v>
@@ -2154,13 +2124,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
         <x:v>63</x:v>
       </x:c>
       <x:c r="D55" s="0" t="n">
-        <x:v>3390</x:v>
+        <x:v>3817</x:v>
       </x:c>
       <x:c r="E55" s="0" t="n">
         <x:v>52</x:v>
@@ -2174,13 +2144,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
       <x:c r="D56" s="0" t="n">
-        <x:v>3685</x:v>
+        <x:v>3870</x:v>
       </x:c>
       <x:c r="E56" s="0" t="n">
         <x:v>52</x:v>
@@ -2194,13 +2164,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
         <x:v>65</x:v>
       </x:c>
       <x:c r="D57" s="0" t="n">
-        <x:v>3685</x:v>
+        <x:v>3986</x:v>
       </x:c>
       <x:c r="E57" s="0" t="n">
         <x:v>52</x:v>
@@ -2214,13 +2184,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
         <x:v>66</x:v>
       </x:c>
       <x:c r="D58" s="0" t="n">
-        <x:v>3759</x:v>
+        <x:v>3990</x:v>
       </x:c>
       <x:c r="E58" s="0" t="n">
         <x:v>52</x:v>
@@ -2234,13 +2204,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
         <x:v>67</x:v>
       </x:c>
       <x:c r="D59" s="0" t="n">
-        <x:v>3817</x:v>
+        <x:v>4238</x:v>
       </x:c>
       <x:c r="E59" s="0" t="n">
         <x:v>52</x:v>
@@ -2254,13 +2224,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
         <x:v>68</x:v>
       </x:c>
       <x:c r="D60" s="0" t="n">
-        <x:v>3900</x:v>
+        <x:v>4350</x:v>
       </x:c>
       <x:c r="E60" s="0" t="n">
         <x:v>52</x:v>
@@ -2274,13 +2244,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
         <x:v>69</x:v>
       </x:c>
       <x:c r="D61" s="0" t="n">
-        <x:v>4450</x:v>
+        <x:v>4577</x:v>
       </x:c>
       <x:c r="E61" s="0" t="n">
         <x:v>52</x:v>
@@ -2294,13 +2264,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
         <x:v>70</x:v>
       </x:c>
       <x:c r="D62" s="0" t="n">
-        <x:v>4779</x:v>
+        <x:v>4769</x:v>
       </x:c>
       <x:c r="E62" s="0" t="n">
         <x:v>52</x:v>
@@ -2314,7 +2284,7 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
         <x:v>71</x:v>
@@ -2334,13 +2304,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
         <x:v>72</x:v>
       </x:c>
       <x:c r="D64" s="0" t="n">
-        <x:v>5350</x:v>
+        <x:v>4879</x:v>
       </x:c>
       <x:c r="E64" s="0" t="n">
         <x:v>52</x:v>
@@ -2354,13 +2324,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
         <x:v>73</x:v>
       </x:c>
       <x:c r="D65" s="0" t="n">
-        <x:v>5450</x:v>
+        <x:v>5084</x:v>
       </x:c>
       <x:c r="E65" s="0" t="n">
         <x:v>52</x:v>
@@ -2374,13 +2344,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
         <x:v>74</x:v>
       </x:c>
       <x:c r="D66" s="0" t="n">
-        <x:v>5490</x:v>
+        <x:v>5220</x:v>
       </x:c>
       <x:c r="E66" s="0" t="n">
         <x:v>52</x:v>
@@ -2394,13 +2364,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
         <x:v>75</x:v>
       </x:c>
       <x:c r="D67" s="0" t="n">
-        <x:v>5519</x:v>
+        <x:v>5338</x:v>
       </x:c>
       <x:c r="E67" s="0" t="n">
         <x:v>52</x:v>
@@ -2414,13 +2384,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
         <x:v>76</x:v>
       </x:c>
       <x:c r="D68" s="0" t="n">
-        <x:v>5580</x:v>
+        <x:v>5350</x:v>
       </x:c>
       <x:c r="E68" s="0" t="n">
         <x:v>52</x:v>
@@ -2434,13 +2404,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
       <x:c r="D69" s="0" t="n">
-        <x:v>5590</x:v>
+        <x:v>5490</x:v>
       </x:c>
       <x:c r="E69" s="0" t="n">
         <x:v>52</x:v>
@@ -2454,13 +2424,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
         <x:v>78</x:v>
       </x:c>
       <x:c r="D70" s="0" t="n">
-        <x:v>5790</x:v>
+        <x:v>5564</x:v>
       </x:c>
       <x:c r="E70" s="0" t="n">
         <x:v>52</x:v>
@@ -2474,13 +2444,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
         <x:v>79</x:v>
       </x:c>
       <x:c r="D71" s="0" t="n">
-        <x:v>5800</x:v>
+        <x:v>5591</x:v>
       </x:c>
       <x:c r="E71" s="0" t="n">
         <x:v>52</x:v>
@@ -2494,13 +2464,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
         <x:v>80</x:v>
       </x:c>
       <x:c r="D72" s="0" t="n">
-        <x:v>5930</x:v>
+        <x:v>5790</x:v>
       </x:c>
       <x:c r="E72" s="0" t="n">
         <x:v>52</x:v>
@@ -2514,13 +2484,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C73" s="0" t="s">
         <x:v>81</x:v>
       </x:c>
       <x:c r="D73" s="0" t="n">
-        <x:v>5968</x:v>
+        <x:v>5800</x:v>
       </x:c>
       <x:c r="E73" s="0" t="n">
         <x:v>52</x:v>
@@ -2534,13 +2504,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
         <x:v>82</x:v>
       </x:c>
       <x:c r="D74" s="0" t="n">
-        <x:v>5968</x:v>
+        <x:v>5860</x:v>
       </x:c>
       <x:c r="E74" s="0" t="n">
         <x:v>52</x:v>
@@ -2554,13 +2524,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
         <x:v>83</x:v>
       </x:c>
       <x:c r="D75" s="0" t="n">
-        <x:v>5990</x:v>
+        <x:v>5960</x:v>
       </x:c>
       <x:c r="E75" s="0" t="n">
         <x:v>52</x:v>
@@ -2574,13 +2544,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
         <x:v>84</x:v>
       </x:c>
       <x:c r="D76" s="0" t="n">
-        <x:v>6096</x:v>
+        <x:v>5968</x:v>
       </x:c>
       <x:c r="E76" s="0" t="n">
         <x:v>52</x:v>
@@ -2594,13 +2564,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C77" s="0" t="s">
         <x:v>85</x:v>
       </x:c>
       <x:c r="D77" s="0" t="n">
-        <x:v>6098</x:v>
+        <x:v>5968</x:v>
       </x:c>
       <x:c r="E77" s="0" t="n">
         <x:v>52</x:v>
@@ -2614,13 +2584,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C78" s="0" t="s">
         <x:v>86</x:v>
       </x:c>
       <x:c r="D78" s="0" t="n">
-        <x:v>6246</x:v>
+        <x:v>5989</x:v>
       </x:c>
       <x:c r="E78" s="0" t="n">
         <x:v>52</x:v>
@@ -2634,13 +2604,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
         <x:v>87</x:v>
       </x:c>
       <x:c r="D79" s="0" t="n">
-        <x:v>6250</x:v>
+        <x:v>6020</x:v>
       </x:c>
       <x:c r="E79" s="0" t="n">
         <x:v>52</x:v>
@@ -2654,13 +2624,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C80" s="0" t="s">
         <x:v>88</x:v>
       </x:c>
       <x:c r="D80" s="0" t="n">
-        <x:v>6425</x:v>
+        <x:v>6093</x:v>
       </x:c>
       <x:c r="E80" s="0" t="n">
         <x:v>52</x:v>
@@ -2674,13 +2644,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
         <x:v>89</x:v>
       </x:c>
       <x:c r="D81" s="0" t="n">
-        <x:v>6430</x:v>
+        <x:v>6096</x:v>
       </x:c>
       <x:c r="E81" s="0" t="n">
         <x:v>52</x:v>
@@ -2694,13 +2664,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C82" s="0" t="s">
         <x:v>90</x:v>
       </x:c>
       <x:c r="D82" s="0" t="n">
-        <x:v>6452</x:v>
+        <x:v>6175</x:v>
       </x:c>
       <x:c r="E82" s="0" t="n">
         <x:v>52</x:v>
@@ -2714,13 +2684,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
         <x:v>91</x:v>
       </x:c>
       <x:c r="D83" s="0" t="n">
-        <x:v>6456</x:v>
+        <x:v>6246</x:v>
       </x:c>
       <x:c r="E83" s="0" t="n">
         <x:v>52</x:v>
@@ -2734,13 +2704,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C84" s="0" t="s">
         <x:v>92</x:v>
       </x:c>
       <x:c r="D84" s="0" t="n">
-        <x:v>6521</x:v>
+        <x:v>6385</x:v>
       </x:c>
       <x:c r="E84" s="0" t="n">
         <x:v>52</x:v>
@@ -2754,13 +2724,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
         <x:v>93</x:v>
       </x:c>
       <x:c r="D85" s="0" t="n">
-        <x:v>6554</x:v>
+        <x:v>6413</x:v>
       </x:c>
       <x:c r="E85" s="0" t="n">
         <x:v>52</x:v>
@@ -2774,13 +2744,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
         <x:v>94</x:v>
       </x:c>
       <x:c r="D86" s="0" t="n">
-        <x:v>6750</x:v>
+        <x:v>6450</x:v>
       </x:c>
       <x:c r="E86" s="0" t="n">
         <x:v>52</x:v>
@@ -2794,13 +2764,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
         <x:v>95</x:v>
       </x:c>
       <x:c r="D87" s="0" t="n">
-        <x:v>6765</x:v>
+        <x:v>6450</x:v>
       </x:c>
       <x:c r="E87" s="0" t="n">
         <x:v>52</x:v>
@@ -2814,13 +2784,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B88" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C88" s="0" t="s">
         <x:v>96</x:v>
       </x:c>
       <x:c r="D88" s="0" t="n">
-        <x:v>6765</x:v>
+        <x:v>6456</x:v>
       </x:c>
       <x:c r="E88" s="0" t="n">
         <x:v>52</x:v>
@@ -2834,13 +2804,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B89" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
         <x:v>97</x:v>
       </x:c>
       <x:c r="D89" s="0" t="n">
-        <x:v>6770</x:v>
+        <x:v>6490</x:v>
       </x:c>
       <x:c r="E89" s="0" t="n">
         <x:v>52</x:v>
@@ -2854,13 +2824,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
         <x:v>98</x:v>
       </x:c>
       <x:c r="D90" s="0" t="n">
-        <x:v>6786</x:v>
+        <x:v>6504</x:v>
       </x:c>
       <x:c r="E90" s="0" t="n">
         <x:v>52</x:v>
@@ -2874,13 +2844,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
         <x:v>99</x:v>
       </x:c>
       <x:c r="D91" s="0" t="n">
-        <x:v>6830</x:v>
+        <x:v>6521</x:v>
       </x:c>
       <x:c r="E91" s="0" t="n">
         <x:v>52</x:v>
@@ -2894,13 +2864,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
         <x:v>100</x:v>
       </x:c>
       <x:c r="D92" s="0" t="n">
-        <x:v>6840</x:v>
+        <x:v>6580</x:v>
       </x:c>
       <x:c r="E92" s="0" t="n">
         <x:v>52</x:v>
@@ -2914,13 +2884,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
         <x:v>101</x:v>
       </x:c>
       <x:c r="D93" s="0" t="n">
-        <x:v>6850</x:v>
+        <x:v>6690</x:v>
       </x:c>
       <x:c r="E93" s="0" t="n">
         <x:v>52</x:v>
@@ -2934,13 +2904,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
         <x:v>102</x:v>
       </x:c>
       <x:c r="D94" s="0" t="n">
-        <x:v>6950</x:v>
+        <x:v>6690</x:v>
       </x:c>
       <x:c r="E94" s="0" t="n">
         <x:v>52</x:v>
@@ -2954,13 +2924,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
         <x:v>103</x:v>
       </x:c>
       <x:c r="D95" s="0" t="n">
-        <x:v>7040</x:v>
+        <x:v>6760</x:v>
       </x:c>
       <x:c r="E95" s="0" t="n">
         <x:v>52</x:v>
@@ -2974,13 +2944,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
         <x:v>104</x:v>
       </x:c>
       <x:c r="D96" s="0" t="n">
-        <x:v>7082</x:v>
+        <x:v>6770</x:v>
       </x:c>
       <x:c r="E96" s="0" t="n">
         <x:v>52</x:v>
@@ -2994,13 +2964,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
         <x:v>105</x:v>
       </x:c>
       <x:c r="D97" s="0" t="n">
-        <x:v>7087</x:v>
+        <x:v>6830</x:v>
       </x:c>
       <x:c r="E97" s="0" t="n">
         <x:v>52</x:v>
@@ -3014,13 +2984,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C98" s="0" t="s">
         <x:v>106</x:v>
       </x:c>
       <x:c r="D98" s="0" t="n">
-        <x:v>7120</x:v>
+        <x:v>6840</x:v>
       </x:c>
       <x:c r="E98" s="0" t="n">
         <x:v>52</x:v>
@@ -3034,13 +3004,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B99" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C99" s="0" t="s">
         <x:v>107</x:v>
       </x:c>
       <x:c r="D99" s="0" t="n">
-        <x:v>7199</x:v>
+        <x:v>6850</x:v>
       </x:c>
       <x:c r="E99" s="0" t="n">
         <x:v>52</x:v>
@@ -3054,13 +3024,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C100" s="0" t="s">
         <x:v>108</x:v>
       </x:c>
       <x:c r="D100" s="0" t="n">
-        <x:v>7213</x:v>
+        <x:v>7003</x:v>
       </x:c>
       <x:c r="E100" s="0" t="n">
         <x:v>52</x:v>
@@ -3074,13 +3044,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B101" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C101" s="0" t="s">
         <x:v>109</x:v>
       </x:c>
       <x:c r="D101" s="0" t="n">
-        <x:v>7230</x:v>
+        <x:v>7079</x:v>
       </x:c>
       <x:c r="E101" s="0" t="n">
         <x:v>52</x:v>
@@ -3094,13 +3064,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B102" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C102" s="0" t="s">
         <x:v>110</x:v>
       </x:c>
       <x:c r="D102" s="0" t="n">
-        <x:v>7245</x:v>
+        <x:v>7090</x:v>
       </x:c>
       <x:c r="E102" s="0" t="n">
         <x:v>52</x:v>
@@ -3114,13 +3084,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B103" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C103" s="0" t="s">
         <x:v>111</x:v>
       </x:c>
       <x:c r="D103" s="0" t="n">
-        <x:v>7250</x:v>
+        <x:v>7150</x:v>
       </x:c>
       <x:c r="E103" s="0" t="n">
         <x:v>52</x:v>
@@ -3134,13 +3104,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B104" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C104" s="0" t="s">
         <x:v>112</x:v>
       </x:c>
       <x:c r="D104" s="0" t="n">
-        <x:v>7270</x:v>
+        <x:v>7155</x:v>
       </x:c>
       <x:c r="E104" s="0" t="n">
         <x:v>52</x:v>
@@ -3154,13 +3124,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B105" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C105" s="0" t="s">
         <x:v>113</x:v>
       </x:c>
       <x:c r="D105" s="0" t="n">
-        <x:v>7290</x:v>
+        <x:v>7200</x:v>
       </x:c>
       <x:c r="E105" s="0" t="n">
         <x:v>52</x:v>
@@ -3174,13 +3144,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B106" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C106" s="0" t="s">
         <x:v>114</x:v>
       </x:c>
       <x:c r="D106" s="0" t="n">
-        <x:v>7290</x:v>
+        <x:v>7213</x:v>
       </x:c>
       <x:c r="E106" s="0" t="n">
         <x:v>52</x:v>
@@ -3194,13 +3164,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B107" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C107" s="0" t="s">
         <x:v>115</x:v>
       </x:c>
       <x:c r="D107" s="0" t="n">
-        <x:v>7290</x:v>
+        <x:v>7260</x:v>
       </x:c>
       <x:c r="E107" s="0" t="n">
         <x:v>52</x:v>
@@ -3214,13 +3184,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B108" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C108" s="0" t="s">
         <x:v>116</x:v>
       </x:c>
       <x:c r="D108" s="0" t="n">
-        <x:v>7490</x:v>
+        <x:v>7290</x:v>
       </x:c>
       <x:c r="E108" s="0" t="n">
         <x:v>52</x:v>
@@ -3234,13 +3204,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B109" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C109" s="0" t="s">
         <x:v>117</x:v>
       </x:c>
       <x:c r="D109" s="0" t="n">
-        <x:v>7660</x:v>
+        <x:v>7290</x:v>
       </x:c>
       <x:c r="E109" s="0" t="n">
         <x:v>52</x:v>
@@ -3254,13 +3224,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B110" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C110" s="0" t="s">
         <x:v>118</x:v>
       </x:c>
       <x:c r="D110" s="0" t="n">
-        <x:v>7690</x:v>
+        <x:v>7290</x:v>
       </x:c>
       <x:c r="E110" s="0" t="n">
         <x:v>52</x:v>
@@ -3274,13 +3244,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B111" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C111" s="0" t="s">
         <x:v>119</x:v>
       </x:c>
       <x:c r="D111" s="0" t="n">
-        <x:v>7707</x:v>
+        <x:v>7290</x:v>
       </x:c>
       <x:c r="E111" s="0" t="n">
         <x:v>52</x:v>
@@ -3294,13 +3264,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B112" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C112" s="0" t="s">
         <x:v>120</x:v>
       </x:c>
       <x:c r="D112" s="0" t="n">
-        <x:v>7860</x:v>
+        <x:v>7487</x:v>
       </x:c>
       <x:c r="E112" s="0" t="n">
         <x:v>52</x:v>
@@ -3314,13 +3284,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B113" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C113" s="0" t="s">
         <x:v>121</x:v>
       </x:c>
       <x:c r="D113" s="0" t="n">
-        <x:v>7969</x:v>
+        <x:v>7613</x:v>
       </x:c>
       <x:c r="E113" s="0" t="n">
         <x:v>52</x:v>
@@ -3334,13 +3304,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B114" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C114" s="0" t="s">
         <x:v>122</x:v>
       </x:c>
       <x:c r="D114" s="0" t="n">
-        <x:v>8056</x:v>
+        <x:v>7629</x:v>
       </x:c>
       <x:c r="E114" s="0" t="n">
         <x:v>52</x:v>
@@ -3354,13 +3324,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B115" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C115" s="0" t="s">
         <x:v>123</x:v>
       </x:c>
       <x:c r="D115" s="0" t="n">
-        <x:v>8131</x:v>
+        <x:v>7648</x:v>
       </x:c>
       <x:c r="E115" s="0" t="n">
         <x:v>52</x:v>
@@ -3374,13 +3344,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B116" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C116" s="0" t="s">
         <x:v>124</x:v>
       </x:c>
       <x:c r="D116" s="0" t="n">
-        <x:v>8150</x:v>
+        <x:v>7660</x:v>
       </x:c>
       <x:c r="E116" s="0" t="n">
         <x:v>52</x:v>
@@ -3394,13 +3364,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B117" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C117" s="0" t="s">
         <x:v>125</x:v>
       </x:c>
       <x:c r="D117" s="0" t="n">
-        <x:v>8170</x:v>
+        <x:v>7690</x:v>
       </x:c>
       <x:c r="E117" s="0" t="n">
         <x:v>52</x:v>
@@ -3411,16 +3381,16 @@
     </x:row>
     <x:row r="118" spans="1:6">
       <x:c r="A118" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B118" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C118" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="D118" s="0" t="n">
-        <x:v>8194</x:v>
+        <x:v>89090</x:v>
       </x:c>
       <x:c r="E118" s="0" t="n">
         <x:v>52</x:v>
@@ -3431,16 +3401,16 @@
     </x:row>
     <x:row r="119" spans="1:6">
       <x:c r="A119" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B119" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C119" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="D119" s="0" t="n">
-        <x:v>8215</x:v>
+        <x:v>97700</x:v>
       </x:c>
       <x:c r="E119" s="0" t="n">
         <x:v>52</x:v>
@@ -3451,16 +3421,16 @@
     </x:row>
     <x:row r="120" spans="1:6">
       <x:c r="A120" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B120" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C120" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="D120" s="0" t="n">
-        <x:v>8215</x:v>
+        <x:v>101879</x:v>
       </x:c>
       <x:c r="E120" s="0" t="n">
         <x:v>52</x:v>
@@ -3471,16 +3441,16 @@
     </x:row>
     <x:row r="121" spans="1:6">
       <x:c r="A121" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B121" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C121" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="D121" s="0" t="n">
-        <x:v>8355</x:v>
+        <x:v>105490</x:v>
       </x:c>
       <x:c r="E121" s="0" t="n">
         <x:v>52</x:v>
@@ -3491,16 +3461,16 @@
     </x:row>
     <x:row r="122" spans="1:6">
       <x:c r="A122" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B122" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C122" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="D122" s="0" t="n">
-        <x:v>8390</x:v>
+        <x:v>109590</x:v>
       </x:c>
       <x:c r="E122" s="0" t="n">
         <x:v>52</x:v>
@@ -3511,16 +3481,16 @@
     </x:row>
     <x:row r="123" spans="1:6">
       <x:c r="A123" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B123" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C123" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="D123" s="0" t="n">
-        <x:v>8480</x:v>
+        <x:v>110013</x:v>
       </x:c>
       <x:c r="E123" s="0" t="n">
         <x:v>52</x:v>
@@ -3531,16 +3501,16 @@
     </x:row>
     <x:row r="124" spans="1:6">
       <x:c r="A124" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="B124" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C124" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="D124" s="0" t="n">
-        <x:v>8481</x:v>
+        <x:v>110886</x:v>
       </x:c>
       <x:c r="E124" s="0" t="n">
         <x:v>52</x:v>
@@ -3554,13 +3524,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B125" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C125" s="0" t="s">
         <x:v>134</x:v>
       </x:c>
       <x:c r="D125" s="0" t="n">
-        <x:v>92890</x:v>
+        <x:v>111050</x:v>
       </x:c>
       <x:c r="E125" s="0" t="n">
         <x:v>52</x:v>
@@ -3574,13 +3544,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B126" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C126" s="0" t="s">
         <x:v>135</x:v>
       </x:c>
       <x:c r="D126" s="0" t="n">
-        <x:v>94320</x:v>
+        <x:v>120650</x:v>
       </x:c>
       <x:c r="E126" s="0" t="n">
         <x:v>52</x:v>
@@ -3594,13 +3564,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B127" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C127" s="0" t="s">
         <x:v>136</x:v>
       </x:c>
       <x:c r="D127" s="0" t="n">
-        <x:v>101943</x:v>
+        <x:v>135190</x:v>
       </x:c>
       <x:c r="E127" s="0" t="n">
         <x:v>52</x:v>
@@ -3614,13 +3584,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B128" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C128" s="0" t="s">
         <x:v>137</x:v>
       </x:c>
       <x:c r="D128" s="0" t="n">
-        <x:v>111523</x:v>
+        <x:v>144015</x:v>
       </x:c>
       <x:c r="E128" s="0" t="n">
         <x:v>52</x:v>
@@ -3634,13 +3604,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B129" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C129" s="0" t="s">
         <x:v>138</x:v>
       </x:c>
       <x:c r="D129" s="0" t="n">
-        <x:v>111800</x:v>
+        <x:v>160390</x:v>
       </x:c>
       <x:c r="E129" s="0" t="n">
         <x:v>52</x:v>
@@ -3651,16 +3621,16 @@
     </x:row>
     <x:row r="130" spans="1:6">
       <x:c r="A130" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B130" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="C130" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D130" s="0" t="n">
-        <x:v>126983</x:v>
+        <x:v>343190</x:v>
       </x:c>
       <x:c r="E130" s="0" t="n">
         <x:v>52</x:v>
@@ -3671,19 +3641,19 @@
     </x:row>
     <x:row r="131" spans="1:6">
       <x:c r="A131" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B131" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C131" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="D131" s="0" t="n">
-        <x:v>127854</x:v>
+        <x:v>138890</x:v>
       </x:c>
       <x:c r="E131" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F131" s="0" t="s">
         <x:v>8</x:v>
@@ -3691,19 +3661,19 @@
     </x:row>
     <x:row r="132" spans="1:6">
       <x:c r="A132" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B132" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C132" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="D132" s="0" t="n">
-        <x:v>144015</x:v>
+        <x:v>139290</x:v>
       </x:c>
       <x:c r="E132" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F132" s="0" t="s">
         <x:v>8</x:v>
@@ -3711,19 +3681,19 @@
     </x:row>
     <x:row r="133" spans="1:6">
       <x:c r="A133" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B133" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C133" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D133" s="0" t="n">
-        <x:v>146477</x:v>
+        <x:v>176390</x:v>
       </x:c>
       <x:c r="E133" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F133" s="0" t="s">
         <x:v>8</x:v>
@@ -3731,19 +3701,19 @@
     </x:row>
     <x:row r="134" spans="1:6">
       <x:c r="A134" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B134" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C134" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="D134" s="0" t="n">
-        <x:v>167690</x:v>
+        <x:v>168990</x:v>
       </x:c>
       <x:c r="E134" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F134" s="0" t="s">
         <x:v>8</x:v>
@@ -3751,19 +3721,19 @@
     </x:row>
     <x:row r="135" spans="1:6">
       <x:c r="A135" s="0" t="n">
-        <x:v>185</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B135" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C135" s="0" t="s">
         <x:v>145</x:v>
       </x:c>
       <x:c r="D135" s="0" t="n">
-        <x:v>309990</x:v>
+        <x:v>144190</x:v>
       </x:c>
       <x:c r="E135" s="0" t="n">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F135" s="0" t="s">
         <x:v>8</x:v>
@@ -3780,7 +3750,7 @@
         <x:v>146</x:v>
       </x:c>
       <x:c r="D136" s="0" t="n">
-        <x:v>129990</x:v>
+        <x:v>196890</x:v>
       </x:c>
       <x:c r="E136" s="0" t="n">
         <x:v>53</x:v>
@@ -3800,7 +3770,7 @@
         <x:v>147</x:v>
       </x:c>
       <x:c r="D137" s="0" t="n">
-        <x:v>131590</x:v>
+        <x:v>220290</x:v>
       </x:c>
       <x:c r="E137" s="0" t="n">
         <x:v>53</x:v>
@@ -3820,7 +3790,7 @@
         <x:v>148</x:v>
       </x:c>
       <x:c r="D138" s="0" t="n">
-        <x:v>133490</x:v>
+        <x:v>197990</x:v>
       </x:c>
       <x:c r="E138" s="0" t="n">
         <x:v>53</x:v>
@@ -3840,7 +3810,7 @@
         <x:v>149</x:v>
       </x:c>
       <x:c r="D139" s="0" t="n">
-        <x:v>138190</x:v>
+        <x:v>138890</x:v>
       </x:c>
       <x:c r="E139" s="0" t="n">
         <x:v>53</x:v>
@@ -3860,7 +3830,7 @@
         <x:v>150</x:v>
       </x:c>
       <x:c r="D140" s="0" t="n">
-        <x:v>139290</x:v>
+        <x:v>152890</x:v>
       </x:c>
       <x:c r="E140" s="0" t="n">
         <x:v>53</x:v>
@@ -3880,7 +3850,7 @@
         <x:v>151</x:v>
       </x:c>
       <x:c r="D141" s="0" t="n">
-        <x:v>139990</x:v>
+        <x:v>202890</x:v>
       </x:c>
       <x:c r="E141" s="0" t="n">
         <x:v>53</x:v>
@@ -3900,7 +3870,7 @@
         <x:v>152</x:v>
       </x:c>
       <x:c r="D142" s="0" t="n">
-        <x:v>142890</x:v>
+        <x:v>210390</x:v>
       </x:c>
       <x:c r="E142" s="0" t="n">
         <x:v>53</x:v>
@@ -3920,7 +3890,7 @@
         <x:v>153</x:v>
       </x:c>
       <x:c r="D143" s="0" t="n">
-        <x:v>144190</x:v>
+        <x:v>185590</x:v>
       </x:c>
       <x:c r="E143" s="0" t="n">
         <x:v>53</x:v>
@@ -3940,7 +3910,7 @@
         <x:v>154</x:v>
       </x:c>
       <x:c r="D144" s="0" t="n">
-        <x:v>146990</x:v>
+        <x:v>174290</x:v>
       </x:c>
       <x:c r="E144" s="0" t="n">
         <x:v>53</x:v>
@@ -3960,7 +3930,7 @@
         <x:v>155</x:v>
       </x:c>
       <x:c r="D145" s="0" t="n">
-        <x:v>149890</x:v>
+        <x:v>133490</x:v>
       </x:c>
       <x:c r="E145" s="0" t="n">
         <x:v>53</x:v>
@@ -3980,7 +3950,7 @@
         <x:v>156</x:v>
       </x:c>
       <x:c r="D146" s="0" t="n">
-        <x:v>152390</x:v>
+        <x:v>169790</x:v>
       </x:c>
       <x:c r="E146" s="0" t="n">
         <x:v>53</x:v>
@@ -4000,7 +3970,7 @@
         <x:v>157</x:v>
       </x:c>
       <x:c r="D147" s="0" t="n">
-        <x:v>160490</x:v>
+        <x:v>202890</x:v>
       </x:c>
       <x:c r="E147" s="0" t="n">
         <x:v>53</x:v>
@@ -4020,7 +3990,7 @@
         <x:v>158</x:v>
       </x:c>
       <x:c r="D148" s="0" t="n">
-        <x:v>163990</x:v>
+        <x:v>224590</x:v>
       </x:c>
       <x:c r="E148" s="0" t="n">
         <x:v>53</x:v>
@@ -4037,10 +4007,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C149" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="D149" s="0" t="n">
-        <x:v>170590</x:v>
+        <x:v>175490</x:v>
       </x:c>
       <x:c r="E149" s="0" t="n">
         <x:v>53</x:v>
@@ -4057,10 +4027,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C150" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D150" s="0" t="n">
-        <x:v>179290</x:v>
+        <x:v>187590</x:v>
       </x:c>
       <x:c r="E150" s="0" t="n">
         <x:v>53</x:v>
@@ -4077,7 +4047,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C151" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="D151" s="0" t="n">
         <x:v>179290</x:v>
@@ -4097,10 +4067,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C152" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="D152" s="0" t="n">
-        <x:v>179390</x:v>
+        <x:v>129990</x:v>
       </x:c>
       <x:c r="E152" s="0" t="n">
         <x:v>53</x:v>
@@ -4117,10 +4087,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C153" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="D153" s="0" t="n">
-        <x:v>179490</x:v>
+        <x:v>132990</x:v>
       </x:c>
       <x:c r="E153" s="0" t="n">
         <x:v>53</x:v>
@@ -4137,10 +4107,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C154" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="D154" s="0" t="n">
-        <x:v>182990</x:v>
+        <x:v>130590</x:v>
       </x:c>
       <x:c r="E154" s="0" t="n">
         <x:v>53</x:v>
@@ -4157,10 +4127,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C155" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="D155" s="0" t="n">
-        <x:v>183290</x:v>
+        <x:v>186790</x:v>
       </x:c>
       <x:c r="E155" s="0" t="n">
         <x:v>53</x:v>
@@ -4177,10 +4147,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C156" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D156" s="0" t="n">
-        <x:v>186890</x:v>
+        <x:v>187590</x:v>
       </x:c>
       <x:c r="E156" s="0" t="n">
         <x:v>53</x:v>
@@ -4197,10 +4167,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C157" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D157" s="0" t="n">
-        <x:v>192390</x:v>
+        <x:v>188090</x:v>
       </x:c>
       <x:c r="E157" s="0" t="n">
         <x:v>53</x:v>
@@ -4217,7 +4187,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C158" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="D158" s="0" t="n">
         <x:v>192690</x:v>
@@ -4237,10 +4207,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C159" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="D159" s="0" t="n">
-        <x:v>195990</x:v>
+        <x:v>196890</x:v>
       </x:c>
       <x:c r="E159" s="0" t="n">
         <x:v>53</x:v>
@@ -4257,10 +4227,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C160" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D160" s="0" t="n">
-        <x:v>204990</x:v>
+        <x:v>197990</x:v>
       </x:c>
       <x:c r="E160" s="0" t="n">
         <x:v>53</x:v>
@@ -4277,10 +4247,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C161" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="D161" s="0" t="n">
-        <x:v>209290</x:v>
+        <x:v>202790</x:v>
       </x:c>
       <x:c r="E161" s="0" t="n">
         <x:v>53</x:v>
@@ -4297,10 +4267,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C162" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="D162" s="0" t="n">
-        <x:v>213190</x:v>
+        <x:v>202890</x:v>
       </x:c>
       <x:c r="E162" s="0" t="n">
         <x:v>53</x:v>
@@ -4317,10 +4287,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C163" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="D163" s="0" t="n">
-        <x:v>213690</x:v>
+        <x:v>202890</x:v>
       </x:c>
       <x:c r="E163" s="0" t="n">
         <x:v>53</x:v>
@@ -4337,10 +4307,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C164" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="D164" s="0" t="n">
-        <x:v>217690</x:v>
+        <x:v>208290</x:v>
       </x:c>
       <x:c r="E164" s="0" t="n">
         <x:v>53</x:v>
@@ -4357,10 +4327,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C165" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D165" s="0" t="n">
-        <x:v>220590</x:v>
+        <x:v>210390</x:v>
       </x:c>
       <x:c r="E165" s="0" t="n">
         <x:v>53</x:v>
@@ -4377,10 +4347,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C166" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D166" s="0" t="n">
-        <x:v>220890</x:v>
+        <x:v>212690</x:v>
       </x:c>
       <x:c r="E166" s="0" t="n">
         <x:v>53</x:v>
@@ -4397,10 +4367,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C167" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D167" s="0" t="n">
-        <x:v>223090</x:v>
+        <x:v>220290</x:v>
       </x:c>
       <x:c r="E167" s="0" t="n">
         <x:v>53</x:v>
@@ -4417,10 +4387,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C168" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="D168" s="0" t="n">
-        <x:v>223190</x:v>
+        <x:v>220890</x:v>
       </x:c>
       <x:c r="E168" s="0" t="n">
         <x:v>53</x:v>
@@ -4437,10 +4407,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C169" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="D169" s="0" t="n">
-        <x:v>260590</x:v>
+        <x:v>224590</x:v>
       </x:c>
       <x:c r="E169" s="0" t="n">
         <x:v>53</x:v>
@@ -4451,16 +4421,16 @@
     </x:row>
     <x:row r="170" spans="1:6">
       <x:c r="A170" s="0" t="n">
-        <x:v>189</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="B170" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C170" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="D170" s="0" t="n">
-        <x:v>16890</x:v>
+        <x:v>234490</x:v>
       </x:c>
       <x:c r="E170" s="0" t="n">
         <x:v>53</x:v>
@@ -4474,13 +4444,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B171" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C171" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D171" s="0" t="n">
-        <x:v>18090</x:v>
+        <x:v>16890</x:v>
       </x:c>
       <x:c r="E171" s="0" t="n">
         <x:v>53</x:v>
@@ -4494,13 +4464,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B172" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C172" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="D172" s="0" t="n">
-        <x:v>19190</x:v>
+        <x:v>19090</x:v>
       </x:c>
       <x:c r="E172" s="0" t="n">
         <x:v>53</x:v>
@@ -4514,13 +4484,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B173" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C173" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="D173" s="0" t="n">
-        <x:v>20490</x:v>
+        <x:v>19390</x:v>
       </x:c>
       <x:c r="E173" s="0" t="n">
         <x:v>53</x:v>
@@ -4534,13 +4504,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B174" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C174" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="D174" s="0" t="n">
-        <x:v>21590</x:v>
+        <x:v>20390</x:v>
       </x:c>
       <x:c r="E174" s="0" t="n">
         <x:v>53</x:v>
@@ -4554,13 +4524,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B175" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C175" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="D175" s="0" t="n">
-        <x:v>22190</x:v>
+        <x:v>21590</x:v>
       </x:c>
       <x:c r="E175" s="0" t="n">
         <x:v>53</x:v>
@@ -4574,13 +4544,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B176" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C176" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="D176" s="0" t="n">
-        <x:v>22890</x:v>
+        <x:v>21690</x:v>
       </x:c>
       <x:c r="E176" s="0" t="n">
         <x:v>53</x:v>
@@ -4594,13 +4564,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B177" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C177" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="D177" s="0" t="n">
-        <x:v>22990</x:v>
+        <x:v>21690</x:v>
       </x:c>
       <x:c r="E177" s="0" t="n">
         <x:v>53</x:v>
@@ -4614,13 +4584,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B178" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="C178" s="0" t="s">
         <x:v>178</x:v>
       </x:c>
-      <x:c r="C178" s="0" t="s">
-        <x:v>186</x:v>
-      </x:c>
       <x:c r="D178" s="0" t="n">
-        <x:v>23590</x:v>
+        <x:v>21990</x:v>
       </x:c>
       <x:c r="E178" s="0" t="n">
         <x:v>53</x:v>
@@ -4634,13 +4604,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B179" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C179" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="D179" s="0" t="n">
-        <x:v>23590</x:v>
+        <x:v>22290</x:v>
       </x:c>
       <x:c r="E179" s="0" t="n">
         <x:v>53</x:v>
@@ -4654,13 +4624,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B180" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C180" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="D180" s="0" t="n">
-        <x:v>23690</x:v>
+        <x:v>22790</x:v>
       </x:c>
       <x:c r="E180" s="0" t="n">
         <x:v>53</x:v>
@@ -4674,13 +4644,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B181" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C181" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="D181" s="0" t="n">
-        <x:v>23790</x:v>
+        <x:v>22790</x:v>
       </x:c>
       <x:c r="E181" s="0" t="n">
         <x:v>53</x:v>
@@ -4694,13 +4664,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B182" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C182" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="D182" s="0" t="n">
-        <x:v>23990</x:v>
+        <x:v>22890</x:v>
       </x:c>
       <x:c r="E182" s="0" t="n">
         <x:v>53</x:v>
@@ -4714,13 +4684,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B183" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C183" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="D183" s="0" t="n">
-        <x:v>23990</x:v>
+        <x:v>22990</x:v>
       </x:c>
       <x:c r="E183" s="0" t="n">
         <x:v>53</x:v>
@@ -4734,13 +4704,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B184" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C184" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="D184" s="0" t="n">
-        <x:v>24190</x:v>
+        <x:v>23490</x:v>
       </x:c>
       <x:c r="E184" s="0" t="n">
         <x:v>53</x:v>
@@ -4754,13 +4724,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B185" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C185" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="D185" s="0" t="n">
-        <x:v>24690</x:v>
+        <x:v>23490</x:v>
       </x:c>
       <x:c r="E185" s="0" t="n">
         <x:v>53</x:v>
@@ -4774,13 +4744,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B186" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C186" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="D186" s="0" t="n">
-        <x:v>24890</x:v>
+        <x:v>23790</x:v>
       </x:c>
       <x:c r="E186" s="0" t="n">
         <x:v>53</x:v>
@@ -4794,13 +4764,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B187" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C187" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="D187" s="0" t="n">
-        <x:v>24990</x:v>
+        <x:v>23990</x:v>
       </x:c>
       <x:c r="E187" s="0" t="n">
         <x:v>53</x:v>
@@ -4814,13 +4784,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B188" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C188" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="D188" s="0" t="n">
-        <x:v>24990</x:v>
+        <x:v>23990</x:v>
       </x:c>
       <x:c r="E188" s="0" t="n">
         <x:v>53</x:v>
@@ -4834,13 +4804,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B189" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C189" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="D189" s="0" t="n">
-        <x:v>25090</x:v>
+        <x:v>24190</x:v>
       </x:c>
       <x:c r="E189" s="0" t="n">
         <x:v>53</x:v>
@@ -4854,13 +4824,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B190" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C190" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="D190" s="0" t="n">
-        <x:v>25190</x:v>
+        <x:v>24190</x:v>
       </x:c>
       <x:c r="E190" s="0" t="n">
         <x:v>53</x:v>
@@ -4874,13 +4844,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B191" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C191" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="D191" s="0" t="n">
-        <x:v>25290</x:v>
+        <x:v>24790</x:v>
       </x:c>
       <x:c r="E191" s="0" t="n">
         <x:v>53</x:v>
@@ -4894,13 +4864,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B192" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C192" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="D192" s="0" t="n">
-        <x:v>25290</x:v>
+        <x:v>24890</x:v>
       </x:c>
       <x:c r="E192" s="0" t="n">
         <x:v>53</x:v>
@@ -4914,13 +4884,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B193" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C193" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="D193" s="0" t="n">
-        <x:v>25490</x:v>
+        <x:v>24990</x:v>
       </x:c>
       <x:c r="E193" s="0" t="n">
         <x:v>53</x:v>
@@ -4934,13 +4904,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B194" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C194" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="D194" s="0" t="n">
-        <x:v>25690</x:v>
+        <x:v>25090</x:v>
       </x:c>
       <x:c r="E194" s="0" t="n">
         <x:v>53</x:v>
@@ -4954,13 +4924,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B195" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C195" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="D195" s="0" t="n">
-        <x:v>26190</x:v>
+        <x:v>25090</x:v>
       </x:c>
       <x:c r="E195" s="0" t="n">
         <x:v>53</x:v>
@@ -4974,13 +4944,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B196" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C196" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="D196" s="0" t="n">
-        <x:v>26290</x:v>
+        <x:v>25290</x:v>
       </x:c>
       <x:c r="E196" s="0" t="n">
         <x:v>53</x:v>
@@ -4994,13 +4964,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B197" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C197" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="D197" s="0" t="n">
-        <x:v>26290</x:v>
+        <x:v>25390</x:v>
       </x:c>
       <x:c r="E197" s="0" t="n">
         <x:v>53</x:v>
@@ -5014,13 +4984,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B198" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C198" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D198" s="0" t="n">
-        <x:v>26390</x:v>
+        <x:v>25490</x:v>
       </x:c>
       <x:c r="E198" s="0" t="n">
         <x:v>53</x:v>
@@ -5034,13 +5004,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B199" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C199" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="D199" s="0" t="n">
-        <x:v>26890</x:v>
+        <x:v>25990</x:v>
       </x:c>
       <x:c r="E199" s="0" t="n">
         <x:v>53</x:v>
@@ -5054,13 +5024,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B200" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C200" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D200" s="0" t="n">
-        <x:v>27290</x:v>
+        <x:v>26090</x:v>
       </x:c>
       <x:c r="E200" s="0" t="n">
         <x:v>53</x:v>
@@ -5074,13 +5044,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B201" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C201" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="D201" s="0" t="n">
-        <x:v>27390</x:v>
+        <x:v>26090</x:v>
       </x:c>
       <x:c r="E201" s="0" t="n">
         <x:v>53</x:v>
@@ -5094,13 +5064,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B202" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C202" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="D202" s="0" t="n">
-        <x:v>27390</x:v>
+        <x:v>26190</x:v>
       </x:c>
       <x:c r="E202" s="0" t="n">
         <x:v>53</x:v>
@@ -5114,13 +5084,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B203" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C203" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="D203" s="0" t="n">
-        <x:v>27390</x:v>
+        <x:v>26190</x:v>
       </x:c>
       <x:c r="E203" s="0" t="n">
         <x:v>53</x:v>
@@ -5134,13 +5104,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B204" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C204" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="D204" s="0" t="n">
-        <x:v>27590</x:v>
+        <x:v>26290</x:v>
       </x:c>
       <x:c r="E204" s="0" t="n">
         <x:v>53</x:v>
@@ -5154,13 +5124,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B205" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C205" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="D205" s="0" t="n">
-        <x:v>28490</x:v>
+        <x:v>26390</x:v>
       </x:c>
       <x:c r="E205" s="0" t="n">
         <x:v>53</x:v>
@@ -5174,13 +5144,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B206" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C206" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="D206" s="0" t="n">
-        <x:v>28490</x:v>
+        <x:v>26490</x:v>
       </x:c>
       <x:c r="E206" s="0" t="n">
         <x:v>53</x:v>
@@ -5194,13 +5164,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B207" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C207" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="D207" s="0" t="n">
-        <x:v>28890</x:v>
+        <x:v>26890</x:v>
       </x:c>
       <x:c r="E207" s="0" t="n">
         <x:v>53</x:v>
@@ -5214,13 +5184,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B208" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C208" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="D208" s="0" t="n">
-        <x:v>29290</x:v>
+        <x:v>27190</x:v>
       </x:c>
       <x:c r="E208" s="0" t="n">
         <x:v>53</x:v>
@@ -5234,13 +5204,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B209" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C209" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="D209" s="0" t="n">
-        <x:v>29790</x:v>
+        <x:v>27290</x:v>
       </x:c>
       <x:c r="E209" s="0" t="n">
         <x:v>53</x:v>
@@ -5254,13 +5224,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B210" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C210" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="D210" s="0" t="n">
-        <x:v>29890</x:v>
+        <x:v>27290</x:v>
       </x:c>
       <x:c r="E210" s="0" t="n">
         <x:v>53</x:v>
@@ -5274,13 +5244,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B211" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C211" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="D211" s="0" t="n">
-        <x:v>29990</x:v>
+        <x:v>27490</x:v>
       </x:c>
       <x:c r="E211" s="0" t="n">
         <x:v>53</x:v>
@@ -5294,13 +5264,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B212" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C212" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="D212" s="0" t="n">
-        <x:v>29990</x:v>
+        <x:v>27590</x:v>
       </x:c>
       <x:c r="E212" s="0" t="n">
         <x:v>53</x:v>
@@ -5314,13 +5284,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B213" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C213" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="D213" s="0" t="n">
-        <x:v>30390</x:v>
+        <x:v>28490</x:v>
       </x:c>
       <x:c r="E213" s="0" t="n">
         <x:v>53</x:v>
@@ -5334,13 +5304,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B214" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C214" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="D214" s="0" t="n">
-        <x:v>30690</x:v>
+        <x:v>28490</x:v>
       </x:c>
       <x:c r="E214" s="0" t="n">
         <x:v>53</x:v>
@@ -5354,13 +5324,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B215" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C215" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="D215" s="0" t="n">
-        <x:v>30790</x:v>
+        <x:v>28890</x:v>
       </x:c>
       <x:c r="E215" s="0" t="n">
         <x:v>53</x:v>
@@ -5374,13 +5344,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B216" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C216" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="D216" s="0" t="n">
-        <x:v>31990</x:v>
+        <x:v>29290</x:v>
       </x:c>
       <x:c r="E216" s="0" t="n">
         <x:v>53</x:v>
@@ -5394,13 +5364,13 @@
         <x:v>189</x:v>
       </x:c>
       <x:c r="B217" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C217" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="D217" s="0" t="n">
-        <x:v>32390</x:v>
+        <x:v>29390</x:v>
       </x:c>
       <x:c r="E217" s="0" t="n">
         <x:v>53</x:v>
@@ -5411,16 +5381,16 @@
     </x:row>
     <x:row r="218" spans="1:6">
       <x:c r="A218" s="0" t="n">
-        <x:v>195</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="B218" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C218" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="D218" s="0" t="n">
-        <x:v>90180</x:v>
+        <x:v>29690</x:v>
       </x:c>
       <x:c r="E218" s="0" t="n">
         <x:v>53</x:v>
@@ -5434,13 +5404,13 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B219" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C219" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="D219" s="0" t="n">
-        <x:v>90180</x:v>
+        <x:v>7290</x:v>
       </x:c>
       <x:c r="E219" s="0" t="n">
         <x:v>53</x:v>
@@ -5454,10 +5424,10 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B220" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C220" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="D220" s="0" t="n">
         <x:v>7690</x:v>
@@ -5474,10 +5444,10 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B221" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C221" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="D221" s="0" t="n">
         <x:v>8090</x:v>
@@ -5494,10 +5464,10 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B222" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C222" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="D222" s="0" t="n">
         <x:v>8990</x:v>
@@ -5514,10 +5484,10 @@
         <x:v>195</x:v>
       </x:c>
       <x:c r="B223" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="C223" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="D223" s="0" t="n">
         <x:v>8990</x:v>
@@ -5534,13 +5504,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B224" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C224" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="D224" s="0" t="n">
-        <x:v>87890</x:v>
+        <x:v>80490</x:v>
       </x:c>
       <x:c r="E224" s="0" t="n">
         <x:v>53</x:v>
@@ -5554,13 +5524,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B225" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C225" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="D225" s="0" t="n">
-        <x:v>88190</x:v>
+        <x:v>84490</x:v>
       </x:c>
       <x:c r="E225" s="0" t="n">
         <x:v>53</x:v>
@@ -5574,13 +5544,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B226" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C226" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="D226" s="0" t="n">
-        <x:v>89990</x:v>
+        <x:v>88990</x:v>
       </x:c>
       <x:c r="E226" s="0" t="n">
         <x:v>53</x:v>
@@ -5594,13 +5564,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B227" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C227" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="D227" s="0" t="n">
-        <x:v>92490</x:v>
+        <x:v>89990</x:v>
       </x:c>
       <x:c r="E227" s="0" t="n">
         <x:v>53</x:v>
@@ -5614,13 +5584,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B228" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C228" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="D228" s="0" t="n">
-        <x:v>92890</x:v>
+        <x:v>94490</x:v>
       </x:c>
       <x:c r="E228" s="0" t="n">
         <x:v>53</x:v>
@@ -5634,13 +5604,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B229" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C229" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D229" s="0" t="n">
-        <x:v>94690</x:v>
+        <x:v>104090</x:v>
       </x:c>
       <x:c r="E229" s="0" t="n">
         <x:v>53</x:v>
@@ -5654,13 +5624,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B230" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C230" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="D230" s="0" t="n">
-        <x:v>129990</x:v>
+        <x:v>109590</x:v>
       </x:c>
       <x:c r="E230" s="0" t="n">
         <x:v>53</x:v>
@@ -5674,13 +5644,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B231" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C231" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="D231" s="0" t="n">
-        <x:v>132990</x:v>
+        <x:v>127390</x:v>
       </x:c>
       <x:c r="E231" s="0" t="n">
         <x:v>53</x:v>
@@ -5694,13 +5664,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B232" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C232" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="D232" s="0" t="n">
-        <x:v>136790</x:v>
+        <x:v>127690</x:v>
       </x:c>
       <x:c r="E232" s="0" t="n">
         <x:v>53</x:v>
@@ -5714,13 +5684,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B233" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C233" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="D233" s="0" t="n">
-        <x:v>143990</x:v>
+        <x:v>147090</x:v>
       </x:c>
       <x:c r="E233" s="0" t="n">
         <x:v>53</x:v>
@@ -5734,13 +5704,13 @@
         <x:v>188</x:v>
       </x:c>
       <x:c r="B234" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C234" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="D234" s="0" t="n">
-        <x:v>148490</x:v>
+        <x:v>154890</x:v>
       </x:c>
       <x:c r="E234" s="0" t="n">
         <x:v>53</x:v>
@@ -5751,16 +5721,16 @@
     </x:row>
     <x:row r="235" spans="1:6">
       <x:c r="A235" s="0" t="n">
-        <x:v>188</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="B235" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="C235" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="D235" s="0" t="n">
-        <x:v>167690</x:v>
+        <x:v>263490</x:v>
       </x:c>
       <x:c r="E235" s="0" t="n">
         <x:v>53</x:v>
@@ -5774,10 +5744,10 @@
         <x:v>185</x:v>
       </x:c>
       <x:c r="B236" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="C236" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="D236" s="0" t="n">
         <x:v>294490</x:v>
@@ -5794,10 +5764,10 @@
         <x:v>185</x:v>
       </x:c>
       <x:c r="B237" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="C237" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="D237" s="0" t="n">
         <x:v>309990</x:v>
@@ -5814,18 +5784,78 @@
         <x:v>186</x:v>
       </x:c>
       <x:c r="B238" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C238" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="D238" s="0" t="n">
-        <x:v>29750</x:v>
+        <x:v>30180</x:v>
       </x:c>
       <x:c r="E238" s="0" t="n">
         <x:v>53</x:v>
       </x:c>
       <x:c r="F238" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="239" spans="1:6">
+      <x:c r="A239" s="0" t="n">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="B239" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="C239" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="D239" s="0" t="n">
+        <x:v>294490</x:v>
+      </x:c>
+      <x:c r="E239" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="F239" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="240" spans="1:6">
+      <x:c r="A240" s="0" t="n">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="B240" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="C240" s="0" t="s">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="D240" s="0" t="n">
+        <x:v>309990</x:v>
+      </x:c>
+      <x:c r="E240" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="F240" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="241" spans="1:6">
+      <x:c r="A241" s="0" t="n">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="B241" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="C241" s="0" t="s">
+        <x:v>222</x:v>
+      </x:c>
+      <x:c r="D241" s="0" t="n">
+        <x:v>30180</x:v>
+      </x:c>
+      <x:c r="E241" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="F241" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>

</xml_diff>